<commit_message>
Reworking + Understanding of RFC Tree, Need to fix accuracy, then utilize Spotify API
</commit_message>
<xml_diff>
--- a/Kpop Songs with Features.xlsx
+++ b/Kpop Songs with Features.xlsx
@@ -684,41 +684,41 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>6TBJkXHPhu3EsMk1bshwuI</t>
+          <t>5yZtAaNMSYxnoP19oSllzU</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.536</v>
+        <v>0.553</v>
       </c>
       <c r="K3" t="n">
-        <v>0.296</v>
+        <v>0.0762</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" t="n">
-        <v>-7.451</v>
+        <v>-14.774</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0346</v>
+        <v>0.0356</v>
       </c>
       <c r="P3" t="n">
-        <v>0.892</v>
+        <v>0.967</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0873</v>
+        <v>0.0704</v>
       </c>
       <c r="S3" t="n">
-        <v>0.151</v>
+        <v>0.243</v>
       </c>
       <c r="T3" t="n">
-        <v>122.907</v>
+        <v>109.759</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
@@ -727,26 +727,26 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>6TBJkXHPhu3EsMk1bshwuI</t>
+          <t>5yZtAaNMSYxnoP19oSllzU</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>spotify:track:6TBJkXHPhu3EsMk1bshwuI</t>
+          <t>spotify:track:5yZtAaNMSYxnoP19oSllzU</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/6TBJkXHPhu3EsMk1bshwuI</t>
+          <t>https://api.spotify.com/v1/tracks/5yZtAaNMSYxnoP19oSllzU</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/6TBJkXHPhu3EsMk1bshwuI</t>
+          <t>https://api.spotify.com/v1/audio-analysis/5yZtAaNMSYxnoP19oSllzU</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>240907</v>
+        <v>272997</v>
       </c>
       <c r="AA3" t="n">
         <v>3</v>
@@ -1594,41 +1594,41 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>380qhTlxvxW5dxseuE9X40</t>
+          <t>0g7ZjaAeHZqoYQ86Q2qBnq</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.182</v>
       </c>
       <c r="K13" t="n">
-        <v>0.226</v>
+        <v>0.0529</v>
       </c>
       <c r="L13" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M13" t="n">
-        <v>-14.411</v>
+        <v>-31.717</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>0.146</v>
+        <v>0.039</v>
       </c>
       <c r="P13" t="n">
-        <v>0.463</v>
+        <v>0.917</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.88</v>
+        <v>0.977</v>
       </c>
       <c r="R13" t="n">
-        <v>0.09420000000000001</v>
+        <v>0.116</v>
       </c>
       <c r="S13" t="n">
-        <v>0.333</v>
+        <v>0.037</v>
       </c>
       <c r="T13" t="n">
-        <v>140.01</v>
+        <v>68.843</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
@@ -1637,26 +1637,26 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>380qhTlxvxW5dxseuE9X40</t>
+          <t>0g7ZjaAeHZqoYQ86Q2qBnq</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>spotify:track:380qhTlxvxW5dxseuE9X40</t>
+          <t>spotify:track:0g7ZjaAeHZqoYQ86Q2qBnq</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/380qhTlxvxW5dxseuE9X40</t>
+          <t>https://api.spotify.com/v1/tracks/0g7ZjaAeHZqoYQ86Q2qBnq</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/380qhTlxvxW5dxseuE9X40</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0g7ZjaAeHZqoYQ86Q2qBnq</t>
         </is>
       </c>
       <c r="Z13" t="n">
-        <v>120000</v>
+        <v>181846</v>
       </c>
       <c r="AA13" t="n">
         <v>4</v>
@@ -2876,41 +2876,41 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>46WaBBaEHzgbN88Ew0nh50</t>
+          <t>49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>0.621</v>
+        <v>0.623</v>
       </c>
       <c r="K27" t="n">
-        <v>0.821</v>
+        <v>0.824</v>
       </c>
       <c r="L27" t="n">
         <v>6</v>
       </c>
       <c r="M27" t="n">
-        <v>-3.662</v>
+        <v>-3.656</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0364</v>
+        <v>0.0384</v>
       </c>
       <c r="P27" t="n">
-        <v>0.00548</v>
+        <v>0.00623</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.000578</v>
+        <v>0.000933</v>
       </c>
       <c r="R27" t="n">
-        <v>0.142</v>
+        <v>0.145</v>
       </c>
       <c r="S27" t="n">
-        <v>0.646</v>
+        <v>0.658</v>
       </c>
       <c r="T27" t="n">
-        <v>120.062</v>
+        <v>120.035</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
@@ -2919,22 +2919,22 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>46WaBBaEHzgbN88Ew0nh50</t>
+          <t>49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>spotify:track:46WaBBaEHzgbN88Ew0nh50</t>
+          <t>spotify:track:49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/46WaBBaEHzgbN88Ew0nh50</t>
+          <t>https://api.spotify.com/v1/tracks/49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/46WaBBaEHzgbN88Ew0nh50</t>
+          <t>https://api.spotify.com/v1/audio-analysis/49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="Z27" t="n">
@@ -4431,41 +4431,41 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
-          <t>4q2HU9Ijpk4zJ24x7oMdXb</t>
+          <t>2EwOnaGCrPjbmyZlt76NN4</t>
         </is>
       </c>
       <c r="J44" t="n">
-        <v>0.867</v>
+        <v>0.866</v>
       </c>
       <c r="K44" t="n">
-        <v>0.783</v>
+        <v>0.738</v>
       </c>
       <c r="L44" t="n">
         <v>11</v>
       </c>
       <c r="M44" t="n">
-        <v>-2.25</v>
+        <v>-3.493</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0687</v>
+        <v>0.0814</v>
       </c>
       <c r="P44" t="n">
-        <v>0.00822</v>
+        <v>0.00615</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.00643</v>
+        <v>0.000549</v>
       </c>
       <c r="R44" t="n">
-        <v>0.302</v>
+        <v>0.227</v>
       </c>
       <c r="S44" t="n">
-        <v>0.701</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="T44" t="n">
-        <v>126.04</v>
+        <v>126.013</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
@@ -4474,26 +4474,26 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>4q2HU9Ijpk4zJ24x7oMdXb</t>
+          <t>2EwOnaGCrPjbmyZlt76NN4</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
         <is>
-          <t>spotify:track:4q2HU9Ijpk4zJ24x7oMdXb</t>
+          <t>spotify:track:2EwOnaGCrPjbmyZlt76NN4</t>
         </is>
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4q2HU9Ijpk4zJ24x7oMdXb</t>
+          <t>https://api.spotify.com/v1/tracks/2EwOnaGCrPjbmyZlt76NN4</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4q2HU9Ijpk4zJ24x7oMdXb</t>
+          <t>https://api.spotify.com/v1/audio-analysis/2EwOnaGCrPjbmyZlt76NN4</t>
         </is>
       </c>
       <c r="Z44" t="n">
-        <v>225373</v>
+        <v>222840</v>
       </c>
       <c r="AA44" t="n">
         <v>4</v>
@@ -6623,41 +6623,41 @@
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
-          <t>46WaBBaEHzgbN88Ew0nh50</t>
+          <t>49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="J68" t="n">
-        <v>0.621</v>
+        <v>0.623</v>
       </c>
       <c r="K68" t="n">
-        <v>0.821</v>
+        <v>0.824</v>
       </c>
       <c r="L68" t="n">
         <v>6</v>
       </c>
       <c r="M68" t="n">
-        <v>-3.662</v>
+        <v>-3.656</v>
       </c>
       <c r="N68" t="n">
         <v>0</v>
       </c>
       <c r="O68" t="n">
-        <v>0.0364</v>
+        <v>0.0384</v>
       </c>
       <c r="P68" t="n">
-        <v>0.00548</v>
+        <v>0.00623</v>
       </c>
       <c r="Q68" t="n">
-        <v>0.000578</v>
+        <v>0.000933</v>
       </c>
       <c r="R68" t="n">
-        <v>0.142</v>
+        <v>0.145</v>
       </c>
       <c r="S68" t="n">
-        <v>0.646</v>
+        <v>0.658</v>
       </c>
       <c r="T68" t="n">
-        <v>120.062</v>
+        <v>120.035</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
@@ -6666,22 +6666,22 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>46WaBBaEHzgbN88Ew0nh50</t>
+          <t>49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
         <is>
-          <t>spotify:track:46WaBBaEHzgbN88Ew0nh50</t>
+          <t>spotify:track:49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/46WaBBaEHzgbN88Ew0nh50</t>
+          <t>https://api.spotify.com/v1/tracks/49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/46WaBBaEHzgbN88Ew0nh50</t>
+          <t>https://api.spotify.com/v1/audio-analysis/49EywdY1mHFj27OY7U8Y2d</t>
         </is>
       </c>
       <c r="Z68" t="n">
@@ -9832,11 +9832,11 @@
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr">
         <is>
-          <t>3CVeGXpoPKJQ9JuhPp3mpL</t>
+          <t>75vepksethG7GrRn815ZYH</t>
         </is>
       </c>
       <c r="J103" t="n">
-        <v>0.613</v>
+        <v>0.614</v>
       </c>
       <c r="K103" t="n">
         <v>0.912</v>
@@ -9845,13 +9845,13 @@
         <v>8</v>
       </c>
       <c r="M103" t="n">
-        <v>-2.464</v>
+        <v>-2.465</v>
       </c>
       <c r="N103" t="n">
         <v>1</v>
       </c>
       <c r="O103" t="n">
-        <v>0.0366</v>
+        <v>0.0367</v>
       </c>
       <c r="P103" t="n">
         <v>0.152</v>
@@ -9863,10 +9863,10 @@
         <v>0.111</v>
       </c>
       <c r="S103" t="n">
-        <v>0.734</v>
+        <v>0.741</v>
       </c>
       <c r="T103" t="n">
-        <v>112.005</v>
+        <v>112.006</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
@@ -9875,22 +9875,22 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>3CVeGXpoPKJQ9JuhPp3mpL</t>
+          <t>75vepksethG7GrRn815ZYH</t>
         </is>
       </c>
       <c r="W103" t="inlineStr">
         <is>
-          <t>spotify:track:3CVeGXpoPKJQ9JuhPp3mpL</t>
+          <t>spotify:track:75vepksethG7GrRn815ZYH</t>
         </is>
       </c>
       <c r="X103" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3CVeGXpoPKJQ9JuhPp3mpL</t>
+          <t>https://api.spotify.com/v1/tracks/75vepksethG7GrRn815ZYH</t>
         </is>
       </c>
       <c r="Y103" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3CVeGXpoPKJQ9JuhPp3mpL</t>
+          <t>https://api.spotify.com/v1/audio-analysis/75vepksethG7GrRn815ZYH</t>
         </is>
       </c>
       <c r="Z103" t="n">
@@ -11561,41 +11561,41 @@
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr">
         <is>
-          <t>52qTle4X9Z5zcThoYR4eY6</t>
+          <t>2UFHMTZyOi9n05pTskkP26</t>
         </is>
       </c>
       <c r="J122" t="n">
-        <v>0.728</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="K122" t="n">
-        <v>0.332</v>
+        <v>0.547</v>
       </c>
       <c r="L122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M122" t="n">
-        <v>-17.488</v>
+        <v>-10.107</v>
       </c>
       <c r="N122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O122" t="n">
-        <v>0.0579</v>
+        <v>0.637</v>
       </c>
       <c r="P122" t="n">
-        <v>0.697</v>
+        <v>0.0371</v>
       </c>
       <c r="Q122" t="n">
-        <v>0.915</v>
+        <v>0</v>
       </c>
       <c r="R122" t="n">
-        <v>0.102</v>
+        <v>0.286</v>
       </c>
       <c r="S122" t="n">
-        <v>0.471</v>
+        <v>0.483</v>
       </c>
       <c r="T122" t="n">
-        <v>114.018</v>
+        <v>77.989</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
@@ -11604,26 +11604,26 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>52qTle4X9Z5zcThoYR4eY6</t>
+          <t>2UFHMTZyOi9n05pTskkP26</t>
         </is>
       </c>
       <c r="W122" t="inlineStr">
         <is>
-          <t>spotify:track:52qTle4X9Z5zcThoYR4eY6</t>
+          <t>spotify:track:2UFHMTZyOi9n05pTskkP26</t>
         </is>
       </c>
       <c r="X122" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/52qTle4X9Z5zcThoYR4eY6</t>
+          <t>https://api.spotify.com/v1/tracks/2UFHMTZyOi9n05pTskkP26</t>
         </is>
       </c>
       <c r="Y122" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/52qTle4X9Z5zcThoYR4eY6</t>
+          <t>https://api.spotify.com/v1/audio-analysis/2UFHMTZyOi9n05pTskkP26</t>
         </is>
       </c>
       <c r="Z122" t="n">
-        <v>140789</v>
+        <v>111067</v>
       </c>
       <c r="AA122" t="n">
         <v>4</v>
@@ -16115,7 +16115,7 @@
       <c r="H172" t="inlineStr"/>
       <c r="I172" t="inlineStr">
         <is>
-          <t>6R6ZoHTypt5lt68MWbzZXv</t>
+          <t>1IWNylpZ477gIVUDpJL66u</t>
         </is>
       </c>
       <c r="J172" t="n">
@@ -16158,22 +16158,22 @@
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>6R6ZoHTypt5lt68MWbzZXv</t>
+          <t>1IWNylpZ477gIVUDpJL66u</t>
         </is>
       </c>
       <c r="W172" t="inlineStr">
         <is>
-          <t>spotify:track:6R6ZoHTypt5lt68MWbzZXv</t>
+          <t>spotify:track:1IWNylpZ477gIVUDpJL66u</t>
         </is>
       </c>
       <c r="X172" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/6R6ZoHTypt5lt68MWbzZXv</t>
+          <t>https://api.spotify.com/v1/tracks/1IWNylpZ477gIVUDpJL66u</t>
         </is>
       </c>
       <c r="Y172" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/6R6ZoHTypt5lt68MWbzZXv</t>
+          <t>https://api.spotify.com/v1/audio-analysis/1IWNylpZ477gIVUDpJL66u</t>
         </is>
       </c>
       <c r="Z172" t="n">
@@ -16570,41 +16570,41 @@
       <c r="H177" t="inlineStr"/>
       <c r="I177" t="inlineStr">
         <is>
-          <t>4gOwpU4kMZZNDWkoHYUj1Z</t>
+          <t>1JNsKjaCFgTxjP3EkKfYZo</t>
         </is>
       </c>
       <c r="J177" t="n">
-        <v>0.702</v>
+        <v>0.875</v>
       </c>
       <c r="K177" t="n">
-        <v>0.837</v>
+        <v>0.526</v>
       </c>
       <c r="L177" t="n">
         <v>5</v>
       </c>
       <c r="M177" t="n">
-        <v>-3.447</v>
+        <v>-6.875</v>
       </c>
       <c r="N177" t="n">
         <v>0</v>
       </c>
       <c r="O177" t="n">
-        <v>0.0567</v>
+        <v>0.232</v>
       </c>
       <c r="P177" t="n">
-        <v>0.0297</v>
+        <v>0.0736</v>
       </c>
       <c r="Q177" t="n">
-        <v>0</v>
+        <v>7.660000000000001e-05</v>
       </c>
       <c r="R177" t="n">
         <v>0.227</v>
       </c>
       <c r="S177" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.672</v>
       </c>
       <c r="T177" t="n">
-        <v>91.986</v>
+        <v>127.976</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
@@ -16613,26 +16613,26 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>4gOwpU4kMZZNDWkoHYUj1Z</t>
+          <t>1JNsKjaCFgTxjP3EkKfYZo</t>
         </is>
       </c>
       <c r="W177" t="inlineStr">
         <is>
-          <t>spotify:track:4gOwpU4kMZZNDWkoHYUj1Z</t>
+          <t>spotify:track:1JNsKjaCFgTxjP3EkKfYZo</t>
         </is>
       </c>
       <c r="X177" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4gOwpU4kMZZNDWkoHYUj1Z</t>
+          <t>https://api.spotify.com/v1/tracks/1JNsKjaCFgTxjP3EkKfYZo</t>
         </is>
       </c>
       <c r="Y177" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4gOwpU4kMZZNDWkoHYUj1Z</t>
+          <t>https://api.spotify.com/v1/audio-analysis/1JNsKjaCFgTxjP3EkKfYZo</t>
         </is>
       </c>
       <c r="Z177" t="n">
-        <v>189680</v>
+        <v>163480</v>
       </c>
       <c r="AA177" t="n">
         <v>4</v>
@@ -18386,41 +18386,41 @@
       <c r="H197" t="inlineStr"/>
       <c r="I197" t="inlineStr">
         <is>
-          <t>2fDfZst43vvbci1jqzrft0</t>
+          <t>0C2gnJXvhtqYiXybFDvOkX</t>
         </is>
       </c>
       <c r="J197" t="n">
-        <v>0.192</v>
+        <v>0.413</v>
       </c>
       <c r="K197" t="n">
-        <v>0.725</v>
+        <v>0.955</v>
       </c>
       <c r="L197" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M197" t="n">
-        <v>-7.864</v>
+        <v>-7.342</v>
       </c>
       <c r="N197" t="n">
         <v>1</v>
       </c>
       <c r="O197" t="n">
-        <v>0.0401</v>
+        <v>0.0391</v>
       </c>
       <c r="P197" t="n">
-        <v>0.509</v>
+        <v>0.0206</v>
       </c>
       <c r="Q197" t="n">
-        <v>0.000129</v>
+        <v>7.96e-05</v>
       </c>
       <c r="R197" t="n">
-        <v>0.882</v>
+        <v>0.209</v>
       </c>
       <c r="S197" t="n">
-        <v>0.298</v>
+        <v>0.451</v>
       </c>
       <c r="T197" t="n">
-        <v>187.158</v>
+        <v>116.192</v>
       </c>
       <c r="U197" t="inlineStr">
         <is>
@@ -18429,26 +18429,26 @@
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>2fDfZst43vvbci1jqzrft0</t>
+          <t>0C2gnJXvhtqYiXybFDvOkX</t>
         </is>
       </c>
       <c r="W197" t="inlineStr">
         <is>
-          <t>spotify:track:2fDfZst43vvbci1jqzrft0</t>
+          <t>spotify:track:0C2gnJXvhtqYiXybFDvOkX</t>
         </is>
       </c>
       <c r="X197" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2fDfZst43vvbci1jqzrft0</t>
+          <t>https://api.spotify.com/v1/tracks/0C2gnJXvhtqYiXybFDvOkX</t>
         </is>
       </c>
       <c r="Y197" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2fDfZst43vvbci1jqzrft0</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0C2gnJXvhtqYiXybFDvOkX</t>
         </is>
       </c>
       <c r="Z197" t="n">
-        <v>259640</v>
+        <v>170440</v>
       </c>
       <c r="AA197" t="n">
         <v>4</v>
@@ -20392,41 +20392,41 @@
       <c r="H219" t="inlineStr"/>
       <c r="I219" t="inlineStr">
         <is>
-          <t>2jL9sjFc2LZsQBGbQnrjXR</t>
+          <t>3LLhE8SrCkXGLjZOFwEhVC</t>
         </is>
       </c>
       <c r="J219" t="n">
-        <v>0.455</v>
+        <v>0.444</v>
       </c>
       <c r="K219" t="n">
-        <v>0.827</v>
+        <v>0.831</v>
       </c>
       <c r="L219" t="n">
         <v>6</v>
       </c>
       <c r="M219" t="n">
-        <v>-1.201</v>
+        <v>-1.2</v>
       </c>
       <c r="N219" t="n">
         <v>1</v>
       </c>
       <c r="O219" t="n">
-        <v>0.0573</v>
+        <v>0.0596</v>
       </c>
       <c r="P219" t="n">
-        <v>0.325</v>
+        <v>0.32</v>
       </c>
       <c r="Q219" t="n">
         <v>0</v>
       </c>
       <c r="R219" t="n">
-        <v>0.0473</v>
+        <v>0.0479</v>
       </c>
       <c r="S219" t="n">
-        <v>0.681</v>
+        <v>0.714</v>
       </c>
       <c r="T219" t="n">
-        <v>169.929</v>
+        <v>169.945</v>
       </c>
       <c r="U219" t="inlineStr">
         <is>
@@ -20435,26 +20435,26 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>2jL9sjFc2LZsQBGbQnrjXR</t>
+          <t>3LLhE8SrCkXGLjZOFwEhVC</t>
         </is>
       </c>
       <c r="W219" t="inlineStr">
         <is>
-          <t>spotify:track:2jL9sjFc2LZsQBGbQnrjXR</t>
+          <t>spotify:track:3LLhE8SrCkXGLjZOFwEhVC</t>
         </is>
       </c>
       <c r="X219" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2jL9sjFc2LZsQBGbQnrjXR</t>
+          <t>https://api.spotify.com/v1/tracks/3LLhE8SrCkXGLjZOFwEhVC</t>
         </is>
       </c>
       <c r="Y219" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2jL9sjFc2LZsQBGbQnrjXR</t>
+          <t>https://api.spotify.com/v1/audio-analysis/3LLhE8SrCkXGLjZOFwEhVC</t>
         </is>
       </c>
       <c r="Z219" t="n">
-        <v>226699</v>
+        <v>226698</v>
       </c>
       <c r="AA219" t="n">
         <v>4</v>
@@ -22129,11 +22129,11 @@
       <c r="H238" t="inlineStr"/>
       <c r="I238" t="inlineStr">
         <is>
-          <t>2Oi0IO8K4BEbhPUdWcjNmv</t>
+          <t>23wVB9x79s921M2Bbu2SB3</t>
         </is>
       </c>
       <c r="J238" t="n">
-        <v>0.642</v>
+        <v>0.643</v>
       </c>
       <c r="K238" t="n">
         <v>0.957</v>
@@ -22163,7 +22163,7 @@
         <v>0.801</v>
       </c>
       <c r="T238" t="n">
-        <v>125.008</v>
+        <v>125.003</v>
       </c>
       <c r="U238" t="inlineStr">
         <is>
@@ -22172,22 +22172,22 @@
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>2Oi0IO8K4BEbhPUdWcjNmv</t>
+          <t>23wVB9x79s921M2Bbu2SB3</t>
         </is>
       </c>
       <c r="W238" t="inlineStr">
         <is>
-          <t>spotify:track:2Oi0IO8K4BEbhPUdWcjNmv</t>
+          <t>spotify:track:23wVB9x79s921M2Bbu2SB3</t>
         </is>
       </c>
       <c r="X238" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2Oi0IO8K4BEbhPUdWcjNmv</t>
+          <t>https://api.spotify.com/v1/tracks/23wVB9x79s921M2Bbu2SB3</t>
         </is>
       </c>
       <c r="Y238" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2Oi0IO8K4BEbhPUdWcjNmv</t>
+          <t>https://api.spotify.com/v1/audio-analysis/23wVB9x79s921M2Bbu2SB3</t>
         </is>
       </c>
       <c r="Z238" t="n">
@@ -26683,41 +26683,41 @@
       <c r="H288" t="inlineStr"/>
       <c r="I288" t="inlineStr">
         <is>
-          <t>296fRjaqLr7ObqVFWK6L8P</t>
+          <t>7y0jebgMdsAEofK2Ye0e6g</t>
         </is>
       </c>
       <c r="J288" t="n">
-        <v>0.605</v>
+        <v>0.669</v>
       </c>
       <c r="K288" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.521</v>
       </c>
       <c r="L288" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M288" t="n">
-        <v>-4.957</v>
+        <v>-5.951</v>
       </c>
       <c r="N288" t="n">
         <v>1</v>
       </c>
       <c r="O288" t="n">
-        <v>0.0419</v>
+        <v>0.0361</v>
       </c>
       <c r="P288" t="n">
-        <v>0.108</v>
+        <v>0.121</v>
       </c>
       <c r="Q288" t="n">
         <v>0</v>
       </c>
       <c r="R288" t="n">
-        <v>0.152</v>
+        <v>0.134</v>
       </c>
       <c r="S288" t="n">
-        <v>0.361</v>
+        <v>0.378</v>
       </c>
       <c r="T288" t="n">
-        <v>154.976</v>
+        <v>90.136</v>
       </c>
       <c r="U288" t="inlineStr">
         <is>
@@ -26726,26 +26726,26 @@
       </c>
       <c r="V288" t="inlineStr">
         <is>
-          <t>296fRjaqLr7ObqVFWK6L8P</t>
+          <t>7y0jebgMdsAEofK2Ye0e6g</t>
         </is>
       </c>
       <c r="W288" t="inlineStr">
         <is>
-          <t>spotify:track:296fRjaqLr7ObqVFWK6L8P</t>
+          <t>spotify:track:7y0jebgMdsAEofK2Ye0e6g</t>
         </is>
       </c>
       <c r="X288" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/296fRjaqLr7ObqVFWK6L8P</t>
+          <t>https://api.spotify.com/v1/tracks/7y0jebgMdsAEofK2Ye0e6g</t>
         </is>
       </c>
       <c r="Y288" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/296fRjaqLr7ObqVFWK6L8P</t>
+          <t>https://api.spotify.com/v1/audio-analysis/7y0jebgMdsAEofK2Ye0e6g</t>
         </is>
       </c>
       <c r="Z288" t="n">
-        <v>208258</v>
+        <v>196771</v>
       </c>
       <c r="AA288" t="n">
         <v>4</v>
@@ -27957,41 +27957,41 @@
       <c r="H302" t="inlineStr"/>
       <c r="I302" t="inlineStr">
         <is>
-          <t>4nJlfdLIucLBkXEJPsSCSp</t>
+          <t>3wWlIamAbDeN1sw7MUKsBG</t>
         </is>
       </c>
       <c r="J302" t="n">
-        <v>0.376</v>
+        <v>0.744</v>
       </c>
       <c r="K302" t="n">
-        <v>0.851</v>
+        <v>0.513</v>
       </c>
       <c r="L302" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M302" t="n">
-        <v>-3.535</v>
+        <v>-8.404</v>
       </c>
       <c r="N302" t="n">
         <v>1</v>
       </c>
       <c r="O302" t="n">
-        <v>0.0459</v>
+        <v>0.0275</v>
       </c>
       <c r="P302" t="n">
-        <v>0.11</v>
+        <v>0.68</v>
       </c>
       <c r="Q302" t="n">
-        <v>0.000124</v>
+        <v>0.000186</v>
       </c>
       <c r="R302" t="n">
-        <v>0.277</v>
+        <v>0.0786</v>
       </c>
       <c r="S302" t="n">
-        <v>0.487</v>
+        <v>0.449</v>
       </c>
       <c r="T302" t="n">
-        <v>173.119</v>
+        <v>93.97</v>
       </c>
       <c r="U302" t="inlineStr">
         <is>
@@ -28000,26 +28000,26 @@
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>4nJlfdLIucLBkXEJPsSCSp</t>
+          <t>3wWlIamAbDeN1sw7MUKsBG</t>
         </is>
       </c>
       <c r="W302" t="inlineStr">
         <is>
-          <t>spotify:track:4nJlfdLIucLBkXEJPsSCSp</t>
+          <t>spotify:track:3wWlIamAbDeN1sw7MUKsBG</t>
         </is>
       </c>
       <c r="X302" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4nJlfdLIucLBkXEJPsSCSp</t>
+          <t>https://api.spotify.com/v1/tracks/3wWlIamAbDeN1sw7MUKsBG</t>
         </is>
       </c>
       <c r="Y302" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4nJlfdLIucLBkXEJPsSCSp</t>
+          <t>https://api.spotify.com/v1/audio-analysis/3wWlIamAbDeN1sw7MUKsBG</t>
         </is>
       </c>
       <c r="Z302" t="n">
-        <v>249533</v>
+        <v>185826</v>
       </c>
       <c r="AA302" t="n">
         <v>4</v>
@@ -28321,41 +28321,41 @@
       <c r="H306" t="inlineStr"/>
       <c r="I306" t="inlineStr">
         <is>
-          <t>6NnCWIWV740gP7DQ8kqdIE</t>
+          <t>0V2passWyAXnON67kfAj7y</t>
         </is>
       </c>
       <c r="J306" t="n">
-        <v>0.726</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="K306" t="n">
-        <v>0.91</v>
+        <v>0.926</v>
       </c>
       <c r="L306" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M306" t="n">
-        <v>-1.948</v>
+        <v>-2.515</v>
       </c>
       <c r="N306" t="n">
         <v>0</v>
       </c>
       <c r="O306" t="n">
-        <v>0.179</v>
+        <v>0.0607</v>
       </c>
       <c r="P306" t="n">
-        <v>0.0413</v>
+        <v>0.0404</v>
       </c>
       <c r="Q306" t="n">
-        <v>7.81e-06</v>
+        <v>0</v>
       </c>
       <c r="R306" t="n">
-        <v>0.479</v>
+        <v>0.19</v>
       </c>
       <c r="S306" t="n">
-        <v>0.648</v>
+        <v>0.86</v>
       </c>
       <c r="T306" t="n">
-        <v>135.966</v>
+        <v>105.969</v>
       </c>
       <c r="U306" t="inlineStr">
         <is>
@@ -28364,26 +28364,26 @@
       </c>
       <c r="V306" t="inlineStr">
         <is>
-          <t>6NnCWIWV740gP7DQ8kqdIE</t>
+          <t>0V2passWyAXnON67kfAj7y</t>
         </is>
       </c>
       <c r="W306" t="inlineStr">
         <is>
-          <t>spotify:track:6NnCWIWV740gP7DQ8kqdIE</t>
+          <t>spotify:track:0V2passWyAXnON67kfAj7y</t>
         </is>
       </c>
       <c r="X306" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/6NnCWIWV740gP7DQ8kqdIE</t>
+          <t>https://api.spotify.com/v1/tracks/0V2passWyAXnON67kfAj7y</t>
         </is>
       </c>
       <c r="Y306" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/6NnCWIWV740gP7DQ8kqdIE</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0V2passWyAXnON67kfAj7y</t>
         </is>
       </c>
       <c r="Z306" t="n">
-        <v>178453</v>
+        <v>162840</v>
       </c>
       <c r="AA306" t="n">
         <v>4</v>
@@ -30145,41 +30145,41 @@
       <c r="H326" t="inlineStr"/>
       <c r="I326" t="inlineStr">
         <is>
-          <t>1d7amkMBfY5jwDaVYpWKUv</t>
+          <t>0Sw5rzQpTmr8Z3QKvuCvhZ</t>
         </is>
       </c>
       <c r="J326" t="n">
-        <v>0.674</v>
+        <v>0.649</v>
       </c>
       <c r="K326" t="n">
-        <v>0.884</v>
+        <v>0.786</v>
       </c>
       <c r="L326" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M326" t="n">
-        <v>-6.062</v>
+        <v>-8.122999999999999</v>
       </c>
       <c r="N326" t="n">
         <v>1</v>
       </c>
       <c r="O326" t="n">
-        <v>0.0988</v>
+        <v>0.116</v>
       </c>
       <c r="P326" t="n">
-        <v>0.0203</v>
+        <v>0.713</v>
       </c>
       <c r="Q326" t="n">
-        <v>0.489</v>
+        <v>0.908</v>
       </c>
       <c r="R326" t="n">
-        <v>0.109</v>
+        <v>0.157</v>
       </c>
       <c r="S326" t="n">
-        <v>0.916</v>
+        <v>0.244</v>
       </c>
       <c r="T326" t="n">
-        <v>101.062</v>
+        <v>181.995</v>
       </c>
       <c r="U326" t="inlineStr">
         <is>
@@ -30188,26 +30188,26 @@
       </c>
       <c r="V326" t="inlineStr">
         <is>
-          <t>1d7amkMBfY5jwDaVYpWKUv</t>
+          <t>0Sw5rzQpTmr8Z3QKvuCvhZ</t>
         </is>
       </c>
       <c r="W326" t="inlineStr">
         <is>
-          <t>spotify:track:1d7amkMBfY5jwDaVYpWKUv</t>
+          <t>spotify:track:0Sw5rzQpTmr8Z3QKvuCvhZ</t>
         </is>
       </c>
       <c r="X326" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/1d7amkMBfY5jwDaVYpWKUv</t>
+          <t>https://api.spotify.com/v1/tracks/0Sw5rzQpTmr8Z3QKvuCvhZ</t>
         </is>
       </c>
       <c r="Y326" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/1d7amkMBfY5jwDaVYpWKUv</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0Sw5rzQpTmr8Z3QKvuCvhZ</t>
         </is>
       </c>
       <c r="Z326" t="n">
-        <v>192961</v>
+        <v>219273</v>
       </c>
       <c r="AA326" t="n">
         <v>4</v>
@@ -30517,41 +30517,41 @@
       <c r="H330" t="inlineStr"/>
       <c r="I330" t="inlineStr">
         <is>
-          <t>4QqROKO0RtV5CvxE7g90uw</t>
+          <t>60VaORSJ5x1D4ZPSc0g2En</t>
         </is>
       </c>
       <c r="J330" t="n">
-        <v>0.706</v>
+        <v>0.438</v>
       </c>
       <c r="K330" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.632</v>
       </c>
       <c r="L330" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M330" t="n">
-        <v>-4.084</v>
+        <v>-4.447</v>
       </c>
       <c r="N330" t="n">
         <v>0</v>
       </c>
       <c r="O330" t="n">
-        <v>0.0483</v>
+        <v>0.0417</v>
       </c>
       <c r="P330" t="n">
-        <v>0.338</v>
+        <v>0.434</v>
       </c>
       <c r="Q330" t="n">
         <v>0</v>
       </c>
       <c r="R330" t="n">
-        <v>0.113</v>
+        <v>0.214</v>
       </c>
       <c r="S330" t="n">
-        <v>0.526</v>
+        <v>0.386</v>
       </c>
       <c r="T330" t="n">
-        <v>136.078</v>
+        <v>61.45</v>
       </c>
       <c r="U330" t="inlineStr">
         <is>
@@ -30560,26 +30560,26 @@
       </c>
       <c r="V330" t="inlineStr">
         <is>
-          <t>4QqROKO0RtV5CvxE7g90uw</t>
+          <t>60VaORSJ5x1D4ZPSc0g2En</t>
         </is>
       </c>
       <c r="W330" t="inlineStr">
         <is>
-          <t>spotify:track:4QqROKO0RtV5CvxE7g90uw</t>
+          <t>spotify:track:60VaORSJ5x1D4ZPSc0g2En</t>
         </is>
       </c>
       <c r="X330" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4QqROKO0RtV5CvxE7g90uw</t>
+          <t>https://api.spotify.com/v1/tracks/60VaORSJ5x1D4ZPSc0g2En</t>
         </is>
       </c>
       <c r="Y330" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4QqROKO0RtV5CvxE7g90uw</t>
+          <t>https://api.spotify.com/v1/audio-analysis/60VaORSJ5x1D4ZPSc0g2En</t>
         </is>
       </c>
       <c r="Z330" t="n">
-        <v>210893</v>
+        <v>213053</v>
       </c>
       <c r="AA330" t="n">
         <v>4</v>
@@ -30608,41 +30608,41 @@
       <c r="H331" t="inlineStr"/>
       <c r="I331" t="inlineStr">
         <is>
-          <t>4slBHMsULWSDtG2hspyTC8</t>
+          <t>25INDjJpGkGwNj970Tjb63</t>
         </is>
       </c>
       <c r="J331" t="n">
-        <v>0.471</v>
+        <v>0.724</v>
       </c>
       <c r="K331" t="n">
-        <v>0.956</v>
+        <v>0.275</v>
       </c>
       <c r="L331" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M331" t="n">
-        <v>-4.696</v>
+        <v>-12.932</v>
       </c>
       <c r="N331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O331" t="n">
-        <v>0.0494</v>
+        <v>0.0573</v>
       </c>
       <c r="P331" t="n">
-        <v>4.52e-06</v>
+        <v>0.518</v>
       </c>
       <c r="Q331" t="n">
-        <v>0.000444</v>
+        <v>0.906</v>
       </c>
       <c r="R331" t="n">
-        <v>0.377</v>
+        <v>0.0949</v>
       </c>
       <c r="S331" t="n">
-        <v>0.551</v>
+        <v>0.462</v>
       </c>
       <c r="T331" t="n">
-        <v>94.976</v>
+        <v>145.91</v>
       </c>
       <c r="U331" t="inlineStr">
         <is>
@@ -30651,26 +30651,26 @@
       </c>
       <c r="V331" t="inlineStr">
         <is>
-          <t>4slBHMsULWSDtG2hspyTC8</t>
+          <t>25INDjJpGkGwNj970Tjb63</t>
         </is>
       </c>
       <c r="W331" t="inlineStr">
         <is>
-          <t>spotify:track:4slBHMsULWSDtG2hspyTC8</t>
+          <t>spotify:track:25INDjJpGkGwNj970Tjb63</t>
         </is>
       </c>
       <c r="X331" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4slBHMsULWSDtG2hspyTC8</t>
+          <t>https://api.spotify.com/v1/tracks/25INDjJpGkGwNj970Tjb63</t>
         </is>
       </c>
       <c r="Y331" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4slBHMsULWSDtG2hspyTC8</t>
+          <t>https://api.spotify.com/v1/audio-analysis/25INDjJpGkGwNj970Tjb63</t>
         </is>
       </c>
       <c r="Z331" t="n">
-        <v>231387</v>
+        <v>65753</v>
       </c>
       <c r="AA331" t="n">
         <v>4</v>
@@ -33975,29 +33975,29 @@
       <c r="H368" t="inlineStr"/>
       <c r="I368" t="inlineStr">
         <is>
-          <t>6x7fux7bZEfnChKx3nhSZn</t>
+          <t>3AtYSKkZ75F7z0fi03pKuq</t>
         </is>
       </c>
       <c r="J368" t="n">
         <v>0.646</v>
       </c>
       <c r="K368" t="n">
-        <v>0.923</v>
+        <v>0.924</v>
       </c>
       <c r="L368" t="n">
         <v>8</v>
       </c>
       <c r="M368" t="n">
-        <v>-1.309</v>
+        <v>-1.302</v>
       </c>
       <c r="N368" t="n">
         <v>1</v>
       </c>
       <c r="O368" t="n">
-        <v>0.0613</v>
+        <v>0.0612</v>
       </c>
       <c r="P368" t="n">
-        <v>0.166</v>
+        <v>0.168</v>
       </c>
       <c r="Q368" t="n">
         <v>0</v>
@@ -34006,10 +34006,10 @@
         <v>0.0507</v>
       </c>
       <c r="S368" t="n">
-        <v>0.703</v>
+        <v>0.706</v>
       </c>
       <c r="T368" t="n">
-        <v>106.086</v>
+        <v>106.087</v>
       </c>
       <c r="U368" t="inlineStr">
         <is>
@@ -34018,22 +34018,22 @@
       </c>
       <c r="V368" t="inlineStr">
         <is>
-          <t>6x7fux7bZEfnChKx3nhSZn</t>
+          <t>3AtYSKkZ75F7z0fi03pKuq</t>
         </is>
       </c>
       <c r="W368" t="inlineStr">
         <is>
-          <t>spotify:track:6x7fux7bZEfnChKx3nhSZn</t>
+          <t>spotify:track:3AtYSKkZ75F7z0fi03pKuq</t>
         </is>
       </c>
       <c r="X368" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/6x7fux7bZEfnChKx3nhSZn</t>
+          <t>https://api.spotify.com/v1/tracks/3AtYSKkZ75F7z0fi03pKuq</t>
         </is>
       </c>
       <c r="Y368" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/6x7fux7bZEfnChKx3nhSZn</t>
+          <t>https://api.spotify.com/v1/audio-analysis/3AtYSKkZ75F7z0fi03pKuq</t>
         </is>
       </c>
       <c r="Z368" t="n">
@@ -34066,7 +34066,7 @@
       <c r="H369" t="inlineStr"/>
       <c r="I369" t="inlineStr">
         <is>
-          <t>2sKWWJ5ee3EnKBztzxPpMH</t>
+          <t>4u04u2pxwZtPKCbURB24GT</t>
         </is>
       </c>
       <c r="J369" t="n">
@@ -34109,22 +34109,22 @@
       </c>
       <c r="V369" t="inlineStr">
         <is>
-          <t>2sKWWJ5ee3EnKBztzxPpMH</t>
+          <t>4u04u2pxwZtPKCbURB24GT</t>
         </is>
       </c>
       <c r="W369" t="inlineStr">
         <is>
-          <t>spotify:track:2sKWWJ5ee3EnKBztzxPpMH</t>
+          <t>spotify:track:4u04u2pxwZtPKCbURB24GT</t>
         </is>
       </c>
       <c r="X369" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2sKWWJ5ee3EnKBztzxPpMH</t>
+          <t>https://api.spotify.com/v1/tracks/4u04u2pxwZtPKCbURB24GT</t>
         </is>
       </c>
       <c r="Y369" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2sKWWJ5ee3EnKBztzxPpMH</t>
+          <t>https://api.spotify.com/v1/audio-analysis/4u04u2pxwZtPKCbURB24GT</t>
         </is>
       </c>
       <c r="Z369" t="n">
@@ -34616,41 +34616,41 @@
       <c r="H375" t="inlineStr"/>
       <c r="I375" t="inlineStr">
         <is>
-          <t>0QGEklEQ3Hm9WlABnHAa5N</t>
+          <t>5gXUFmE5AKFiInKyHVVEnL</t>
         </is>
       </c>
       <c r="J375" t="n">
-        <v>0.708</v>
+        <v>0.606</v>
       </c>
       <c r="K375" t="n">
-        <v>0.907</v>
+        <v>0.623</v>
       </c>
       <c r="L375" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M375" t="n">
-        <v>-4.935</v>
+        <v>-4.01</v>
       </c>
       <c r="N375" t="n">
         <v>1</v>
       </c>
       <c r="O375" t="n">
-        <v>0.0786</v>
+        <v>0.0414</v>
       </c>
       <c r="P375" t="n">
-        <v>0.439</v>
+        <v>0.358</v>
       </c>
       <c r="Q375" t="n">
-        <v>0</v>
+        <v>6.13e-06</v>
       </c>
       <c r="R375" t="n">
-        <v>0.0922</v>
+        <v>0.0716</v>
       </c>
       <c r="S375" t="n">
-        <v>0.712</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="T375" t="n">
-        <v>117.987</v>
+        <v>99.48699999999999</v>
       </c>
       <c r="U375" t="inlineStr">
         <is>
@@ -34659,26 +34659,26 @@
       </c>
       <c r="V375" t="inlineStr">
         <is>
-          <t>0QGEklEQ3Hm9WlABnHAa5N</t>
+          <t>5gXUFmE5AKFiInKyHVVEnL</t>
         </is>
       </c>
       <c r="W375" t="inlineStr">
         <is>
-          <t>spotify:track:0QGEklEQ3Hm9WlABnHAa5N</t>
+          <t>spotify:track:5gXUFmE5AKFiInKyHVVEnL</t>
         </is>
       </c>
       <c r="X375" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/0QGEklEQ3Hm9WlABnHAa5N</t>
+          <t>https://api.spotify.com/v1/tracks/5gXUFmE5AKFiInKyHVVEnL</t>
         </is>
       </c>
       <c r="Y375" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/0QGEklEQ3Hm9WlABnHAa5N</t>
+          <t>https://api.spotify.com/v1/audio-analysis/5gXUFmE5AKFiInKyHVVEnL</t>
         </is>
       </c>
       <c r="Z375" t="n">
-        <v>256867</v>
+        <v>180427</v>
       </c>
       <c r="AA375" t="n">
         <v>4</v>
@@ -35071,41 +35071,41 @@
       <c r="H380" t="inlineStr"/>
       <c r="I380" t="inlineStr">
         <is>
-          <t>3G1aAxWS2Nd17FQs4PWV6X</t>
+          <t>69xohKu8C1fsflYAiSNbwM</t>
         </is>
       </c>
       <c r="J380" t="n">
-        <v>0.554</v>
+        <v>0.724</v>
       </c>
       <c r="K380" t="n">
-        <v>0.878</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="L380" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M380" t="n">
-        <v>-3.02</v>
+        <v>-3.747</v>
       </c>
       <c r="N380" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O380" t="n">
-        <v>0.0513</v>
+        <v>0.168</v>
       </c>
       <c r="P380" t="n">
-        <v>0.00146</v>
+        <v>0.0201</v>
       </c>
       <c r="Q380" t="n">
         <v>0</v>
       </c>
       <c r="R380" t="n">
-        <v>0.0998</v>
+        <v>0.0358</v>
       </c>
       <c r="S380" t="n">
-        <v>0.55</v>
+        <v>0.696</v>
       </c>
       <c r="T380" t="n">
-        <v>132.896</v>
+        <v>77.004</v>
       </c>
       <c r="U380" t="inlineStr">
         <is>
@@ -35114,26 +35114,26 @@
       </c>
       <c r="V380" t="inlineStr">
         <is>
-          <t>3G1aAxWS2Nd17FQs4PWV6X</t>
+          <t>69xohKu8C1fsflYAiSNbwM</t>
         </is>
       </c>
       <c r="W380" t="inlineStr">
         <is>
-          <t>spotify:track:3G1aAxWS2Nd17FQs4PWV6X</t>
+          <t>spotify:track:69xohKu8C1fsflYAiSNbwM</t>
         </is>
       </c>
       <c r="X380" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3G1aAxWS2Nd17FQs4PWV6X</t>
+          <t>https://api.spotify.com/v1/tracks/69xohKu8C1fsflYAiSNbwM</t>
         </is>
       </c>
       <c r="Y380" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3G1aAxWS2Nd17FQs4PWV6X</t>
+          <t>https://api.spotify.com/v1/audio-analysis/69xohKu8C1fsflYAiSNbwM</t>
         </is>
       </c>
       <c r="Z380" t="n">
-        <v>236748</v>
+        <v>204940</v>
       </c>
       <c r="AA380" t="n">
         <v>4</v>
@@ -35617,41 +35617,41 @@
       <c r="H386" t="inlineStr"/>
       <c r="I386" t="inlineStr">
         <is>
-          <t>4ugyTyklumfcYWf2JBkmgx</t>
+          <t>3iEd0mTmjBWRm2l4McR0Mm</t>
         </is>
       </c>
       <c r="J386" t="n">
-        <v>0.57</v>
+        <v>0.535</v>
       </c>
       <c r="K386" t="n">
-        <v>0.761</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="L386" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M386" t="n">
-        <v>-5.506</v>
+        <v>-5.964</v>
       </c>
       <c r="N386" t="n">
         <v>1</v>
       </c>
       <c r="O386" t="n">
-        <v>0.0271</v>
+        <v>0.106</v>
       </c>
       <c r="P386" t="n">
-        <v>0.182</v>
+        <v>0.0138</v>
       </c>
       <c r="Q386" t="n">
-        <v>0.000128</v>
+        <v>0</v>
       </c>
       <c r="R386" t="n">
-        <v>0.102</v>
+        <v>0.64</v>
       </c>
       <c r="S386" t="n">
-        <v>0.745</v>
+        <v>0.468</v>
       </c>
       <c r="T386" t="n">
-        <v>100.988</v>
+        <v>159.911</v>
       </c>
       <c r="U386" t="inlineStr">
         <is>
@@ -35660,26 +35660,26 @@
       </c>
       <c r="V386" t="inlineStr">
         <is>
-          <t>4ugyTyklumfcYWf2JBkmgx</t>
+          <t>3iEd0mTmjBWRm2l4McR0Mm</t>
         </is>
       </c>
       <c r="W386" t="inlineStr">
         <is>
-          <t>spotify:track:4ugyTyklumfcYWf2JBkmgx</t>
+          <t>spotify:track:3iEd0mTmjBWRm2l4McR0Mm</t>
         </is>
       </c>
       <c r="X386" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4ugyTyklumfcYWf2JBkmgx</t>
+          <t>https://api.spotify.com/v1/tracks/3iEd0mTmjBWRm2l4McR0Mm</t>
         </is>
       </c>
       <c r="Y386" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4ugyTyklumfcYWf2JBkmgx</t>
+          <t>https://api.spotify.com/v1/audio-analysis/3iEd0mTmjBWRm2l4McR0Mm</t>
         </is>
       </c>
       <c r="Z386" t="n">
-        <v>194133</v>
+        <v>209792</v>
       </c>
       <c r="AA386" t="n">
         <v>4</v>
@@ -36254,41 +36254,41 @@
       <c r="H393" t="inlineStr"/>
       <c r="I393" t="inlineStr">
         <is>
-          <t>2P3wBy0Ljm2URED3zczeMr</t>
+          <t>1H7AvyWHYAYvbjFi1IVUhP</t>
         </is>
       </c>
       <c r="J393" t="n">
-        <v>0.881</v>
+        <v>0.632</v>
       </c>
       <c r="K393" t="n">
-        <v>0.744</v>
+        <v>0.914</v>
       </c>
       <c r="L393" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M393" t="n">
-        <v>-3.502</v>
+        <v>-3.513</v>
       </c>
       <c r="N393" t="n">
         <v>1</v>
       </c>
       <c r="O393" t="n">
-        <v>0.184</v>
+        <v>0.142</v>
       </c>
       <c r="P393" t="n">
-        <v>0.147</v>
+        <v>0.00339</v>
       </c>
       <c r="Q393" t="n">
         <v>0</v>
       </c>
       <c r="R393" t="n">
-        <v>0.058</v>
+        <v>0.134</v>
       </c>
       <c r="S393" t="n">
-        <v>0.766</v>
+        <v>0.591</v>
       </c>
       <c r="T393" t="n">
-        <v>130.044</v>
+        <v>134.899</v>
       </c>
       <c r="U393" t="inlineStr">
         <is>
@@ -36297,26 +36297,26 @@
       </c>
       <c r="V393" t="inlineStr">
         <is>
-          <t>2P3wBy0Ljm2URED3zczeMr</t>
+          <t>1H7AvyWHYAYvbjFi1IVUhP</t>
         </is>
       </c>
       <c r="W393" t="inlineStr">
         <is>
-          <t>spotify:track:2P3wBy0Ljm2URED3zczeMr</t>
+          <t>spotify:track:1H7AvyWHYAYvbjFi1IVUhP</t>
         </is>
       </c>
       <c r="X393" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2P3wBy0Ljm2URED3zczeMr</t>
+          <t>https://api.spotify.com/v1/tracks/1H7AvyWHYAYvbjFi1IVUhP</t>
         </is>
       </c>
       <c r="Y393" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2P3wBy0Ljm2URED3zczeMr</t>
+          <t>https://api.spotify.com/v1/audio-analysis/1H7AvyWHYAYvbjFi1IVUhP</t>
         </is>
       </c>
       <c r="Z393" t="n">
-        <v>183747</v>
+        <v>193399</v>
       </c>
       <c r="AA393" t="n">
         <v>4</v>
@@ -38165,41 +38165,41 @@
       <c r="H414" t="inlineStr"/>
       <c r="I414" t="inlineStr">
         <is>
-          <t>0XpL0wNViYINLsrerkNggK</t>
+          <t>3MyuNo54MhCTpzzHNPqRpn</t>
         </is>
       </c>
       <c r="J414" t="n">
-        <v>0.646</v>
+        <v>0.53</v>
       </c>
       <c r="K414" t="n">
-        <v>0.411</v>
+        <v>0.968</v>
       </c>
       <c r="L414" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M414" t="n">
-        <v>-15.416</v>
+        <v>-3.941</v>
       </c>
       <c r="N414" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O414" t="n">
-        <v>0.163</v>
+        <v>0.07530000000000001</v>
       </c>
       <c r="P414" t="n">
-        <v>0.312</v>
+        <v>0.000702</v>
       </c>
       <c r="Q414" t="n">
-        <v>0.79</v>
+        <v>0.0118</v>
       </c>
       <c r="R414" t="n">
-        <v>0.11</v>
+        <v>0.228</v>
       </c>
       <c r="S414" t="n">
-        <v>0.315</v>
+        <v>0.338</v>
       </c>
       <c r="T414" t="n">
-        <v>110.199</v>
+        <v>110.974</v>
       </c>
       <c r="U414" t="inlineStr">
         <is>
@@ -38208,26 +38208,26 @@
       </c>
       <c r="V414" t="inlineStr">
         <is>
-          <t>0XpL0wNViYINLsrerkNggK</t>
+          <t>3MyuNo54MhCTpzzHNPqRpn</t>
         </is>
       </c>
       <c r="W414" t="inlineStr">
         <is>
-          <t>spotify:track:0XpL0wNViYINLsrerkNggK</t>
+          <t>spotify:track:3MyuNo54MhCTpzzHNPqRpn</t>
         </is>
       </c>
       <c r="X414" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/0XpL0wNViYINLsrerkNggK</t>
+          <t>https://api.spotify.com/v1/tracks/3MyuNo54MhCTpzzHNPqRpn</t>
         </is>
       </c>
       <c r="Y414" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/0XpL0wNViYINLsrerkNggK</t>
+          <t>https://api.spotify.com/v1/audio-analysis/3MyuNo54MhCTpzzHNPqRpn</t>
         </is>
       </c>
       <c r="Z414" t="n">
-        <v>82731</v>
+        <v>289920</v>
       </c>
       <c r="AA414" t="n">
         <v>4</v>
@@ -40353,41 +40353,41 @@
       <c r="H438" t="inlineStr"/>
       <c r="I438" t="inlineStr">
         <is>
-          <t>7AKKUOFQjjhFyjzvhtawsM</t>
+          <t>0U9jNoTJeTxXToakhsb7pV</t>
         </is>
       </c>
       <c r="J438" t="n">
-        <v>0.436</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="K438" t="n">
-        <v>0.832</v>
+        <v>0.888</v>
       </c>
       <c r="L438" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M438" t="n">
-        <v>-3.243</v>
+        <v>-2.725</v>
       </c>
       <c r="N438" t="n">
         <v>0</v>
       </c>
       <c r="O438" t="n">
-        <v>0.326</v>
+        <v>0.146</v>
       </c>
       <c r="P438" t="n">
-        <v>0.041</v>
+        <v>0.0596</v>
       </c>
       <c r="Q438" t="n">
-        <v>5.8e-05</v>
+        <v>2.14e-05</v>
       </c>
       <c r="R438" t="n">
-        <v>0.803</v>
+        <v>0.181</v>
       </c>
       <c r="S438" t="n">
-        <v>0.651</v>
+        <v>0.791</v>
       </c>
       <c r="T438" t="n">
-        <v>167.024</v>
+        <v>64.92700000000001</v>
       </c>
       <c r="U438" t="inlineStr">
         <is>
@@ -40396,26 +40396,26 @@
       </c>
       <c r="V438" t="inlineStr">
         <is>
-          <t>7AKKUOFQjjhFyjzvhtawsM</t>
+          <t>0U9jNoTJeTxXToakhsb7pV</t>
         </is>
       </c>
       <c r="W438" t="inlineStr">
         <is>
-          <t>spotify:track:7AKKUOFQjjhFyjzvhtawsM</t>
+          <t>spotify:track:0U9jNoTJeTxXToakhsb7pV</t>
         </is>
       </c>
       <c r="X438" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/7AKKUOFQjjhFyjzvhtawsM</t>
+          <t>https://api.spotify.com/v1/tracks/0U9jNoTJeTxXToakhsb7pV</t>
         </is>
       </c>
       <c r="Y438" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/7AKKUOFQjjhFyjzvhtawsM</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0U9jNoTJeTxXToakhsb7pV</t>
         </is>
       </c>
       <c r="Z438" t="n">
-        <v>165160</v>
+        <v>201920</v>
       </c>
       <c r="AA438" t="n">
         <v>4</v>
@@ -41900,41 +41900,41 @@
       <c r="H455" t="inlineStr"/>
       <c r="I455" t="inlineStr">
         <is>
-          <t>5xhiAP5eWI9PKh9UZk7YNV</t>
+          <t>5vCXnSlbAEkuJ3w2O0ALan</t>
         </is>
       </c>
       <c r="J455" t="n">
-        <v>0.767</v>
+        <v>0.709</v>
       </c>
       <c r="K455" t="n">
-        <v>0.479</v>
+        <v>0.639</v>
       </c>
       <c r="L455" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M455" t="n">
-        <v>-6.156</v>
+        <v>-7.063</v>
       </c>
       <c r="N455" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O455" t="n">
-        <v>0.28</v>
+        <v>0.0399</v>
       </c>
       <c r="P455" t="n">
-        <v>0.102</v>
+        <v>0.00244</v>
       </c>
       <c r="Q455" t="n">
-        <v>0</v>
+        <v>0.0697</v>
       </c>
       <c r="R455" t="n">
-        <v>0.125</v>
+        <v>0.08649999999999999</v>
       </c>
       <c r="S455" t="n">
-        <v>0.252</v>
+        <v>0.439</v>
       </c>
       <c r="T455" t="n">
-        <v>140.031</v>
+        <v>135.013</v>
       </c>
       <c r="U455" t="inlineStr">
         <is>
@@ -41943,26 +41943,26 @@
       </c>
       <c r="V455" t="inlineStr">
         <is>
-          <t>5xhiAP5eWI9PKh9UZk7YNV</t>
+          <t>5vCXnSlbAEkuJ3w2O0ALan</t>
         </is>
       </c>
       <c r="W455" t="inlineStr">
         <is>
-          <t>spotify:track:5xhiAP5eWI9PKh9UZk7YNV</t>
+          <t>spotify:track:5vCXnSlbAEkuJ3w2O0ALan</t>
         </is>
       </c>
       <c r="X455" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/5xhiAP5eWI9PKh9UZk7YNV</t>
+          <t>https://api.spotify.com/v1/tracks/5vCXnSlbAEkuJ3w2O0ALan</t>
         </is>
       </c>
       <c r="Y455" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/5xhiAP5eWI9PKh9UZk7YNV</t>
+          <t>https://api.spotify.com/v1/audio-analysis/5vCXnSlbAEkuJ3w2O0ALan</t>
         </is>
       </c>
       <c r="Z455" t="n">
-        <v>110052</v>
+        <v>194587</v>
       </c>
       <c r="AA455" t="n">
         <v>4</v>
@@ -42173,41 +42173,41 @@
       <c r="H458" t="inlineStr"/>
       <c r="I458" t="inlineStr">
         <is>
-          <t>3l3wUDDHEAqOUTSAACKL8b</t>
+          <t>2tDOCMuKSX9IEo9TJ4pBBk</t>
         </is>
       </c>
       <c r="J458" t="n">
-        <v>0.887</v>
+        <v>0.902</v>
       </c>
       <c r="K458" t="n">
-        <v>0.647</v>
+        <v>0.527</v>
       </c>
       <c r="L458" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M458" t="n">
-        <v>-3.851</v>
+        <v>-6.448</v>
       </c>
       <c r="N458" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O458" t="n">
-        <v>0.0582</v>
+        <v>0.249</v>
       </c>
       <c r="P458" t="n">
-        <v>0.0688</v>
+        <v>0.14</v>
       </c>
       <c r="Q458" t="n">
-        <v>0</v>
+        <v>3.17e-06</v>
       </c>
       <c r="R458" t="n">
-        <v>0.0429</v>
+        <v>0.0959</v>
       </c>
       <c r="S458" t="n">
-        <v>0.863</v>
+        <v>0.763</v>
       </c>
       <c r="T458" t="n">
-        <v>104.981</v>
+        <v>100.037</v>
       </c>
       <c r="U458" t="inlineStr">
         <is>
@@ -42216,26 +42216,26 @@
       </c>
       <c r="V458" t="inlineStr">
         <is>
-          <t>3l3wUDDHEAqOUTSAACKL8b</t>
+          <t>2tDOCMuKSX9IEo9TJ4pBBk</t>
         </is>
       </c>
       <c r="W458" t="inlineStr">
         <is>
-          <t>spotify:track:3l3wUDDHEAqOUTSAACKL8b</t>
+          <t>spotify:track:2tDOCMuKSX9IEo9TJ4pBBk</t>
         </is>
       </c>
       <c r="X458" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3l3wUDDHEAqOUTSAACKL8b</t>
+          <t>https://api.spotify.com/v1/tracks/2tDOCMuKSX9IEo9TJ4pBBk</t>
         </is>
       </c>
       <c r="Y458" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3l3wUDDHEAqOUTSAACKL8b</t>
+          <t>https://api.spotify.com/v1/audio-analysis/2tDOCMuKSX9IEo9TJ4pBBk</t>
         </is>
       </c>
       <c r="Z458" t="n">
-        <v>186323</v>
+        <v>99280</v>
       </c>
       <c r="AA458" t="n">
         <v>4</v>
@@ -42446,41 +42446,41 @@
       <c r="H461" t="inlineStr"/>
       <c r="I461" t="inlineStr">
         <is>
-          <t>3QI9dQGIpc5HpAyHhXYZJd</t>
+          <t>4cyVnu1W88UuIdNusX8D1A</t>
         </is>
       </c>
       <c r="J461" t="n">
-        <v>0.734</v>
+        <v>0.68</v>
       </c>
       <c r="K461" t="n">
-        <v>0.454</v>
+        <v>0.904</v>
       </c>
       <c r="L461" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M461" t="n">
-        <v>-7.305</v>
+        <v>-2.056</v>
       </c>
       <c r="N461" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O461" t="n">
-        <v>0.355</v>
+        <v>0.117</v>
       </c>
       <c r="P461" t="n">
-        <v>0.145</v>
+        <v>0.287</v>
       </c>
       <c r="Q461" t="n">
         <v>0</v>
       </c>
       <c r="R461" t="n">
-        <v>0.122</v>
+        <v>0.103</v>
       </c>
       <c r="S461" t="n">
-        <v>0.253</v>
+        <v>0.602</v>
       </c>
       <c r="T461" t="n">
-        <v>140.294</v>
+        <v>117.995</v>
       </c>
       <c r="U461" t="inlineStr">
         <is>
@@ -42489,26 +42489,26 @@
       </c>
       <c r="V461" t="inlineStr">
         <is>
-          <t>3QI9dQGIpc5HpAyHhXYZJd</t>
+          <t>4cyVnu1W88UuIdNusX8D1A</t>
         </is>
       </c>
       <c r="W461" t="inlineStr">
         <is>
-          <t>spotify:track:3QI9dQGIpc5HpAyHhXYZJd</t>
+          <t>spotify:track:4cyVnu1W88UuIdNusX8D1A</t>
         </is>
       </c>
       <c r="X461" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3QI9dQGIpc5HpAyHhXYZJd</t>
+          <t>https://api.spotify.com/v1/tracks/4cyVnu1W88UuIdNusX8D1A</t>
         </is>
       </c>
       <c r="Y461" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3QI9dQGIpc5HpAyHhXYZJd</t>
+          <t>https://api.spotify.com/v1/audio-analysis/4cyVnu1W88UuIdNusX8D1A</t>
         </is>
       </c>
       <c r="Z461" t="n">
-        <v>125005</v>
+        <v>202107</v>
       </c>
       <c r="AA461" t="n">
         <v>4</v>
@@ -43546,41 +43546,41 @@
       <c r="H473" t="inlineStr"/>
       <c r="I473" t="inlineStr">
         <is>
-          <t>2H30WL3exSctlDC9GyRbD4</t>
+          <t>2DkZisoN9h1dLa8Sn5sx0n</t>
         </is>
       </c>
       <c r="J473" t="n">
-        <v>0.496</v>
+        <v>0.203</v>
       </c>
       <c r="K473" t="n">
-        <v>0.644</v>
+        <v>0.715</v>
       </c>
       <c r="L473" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M473" t="n">
-        <v>-5.385</v>
+        <v>-5.485</v>
       </c>
       <c r="N473" t="n">
         <v>1</v>
       </c>
       <c r="O473" t="n">
-        <v>0.0269</v>
+        <v>0.0494</v>
       </c>
       <c r="P473" t="n">
-        <v>0.264</v>
+        <v>0.0487</v>
       </c>
       <c r="Q473" t="n">
-        <v>0</v>
+        <v>0.00082</v>
       </c>
       <c r="R473" t="n">
-        <v>0.06950000000000001</v>
+        <v>0.051</v>
       </c>
       <c r="S473" t="n">
-        <v>0.435</v>
+        <v>0.327</v>
       </c>
       <c r="T473" t="n">
-        <v>96.017</v>
+        <v>78.554</v>
       </c>
       <c r="U473" t="inlineStr">
         <is>
@@ -43589,29 +43589,29 @@
       </c>
       <c r="V473" t="inlineStr">
         <is>
-          <t>2H30WL3exSctlDC9GyRbD4</t>
+          <t>2DkZisoN9h1dLa8Sn5sx0n</t>
         </is>
       </c>
       <c r="W473" t="inlineStr">
         <is>
-          <t>spotify:track:2H30WL3exSctlDC9GyRbD4</t>
+          <t>spotify:track:2DkZisoN9h1dLa8Sn5sx0n</t>
         </is>
       </c>
       <c r="X473" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2H30WL3exSctlDC9GyRbD4</t>
+          <t>https://api.spotify.com/v1/tracks/2DkZisoN9h1dLa8Sn5sx0n</t>
         </is>
       </c>
       <c r="Y473" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2H30WL3exSctlDC9GyRbD4</t>
+          <t>https://api.spotify.com/v1/audio-analysis/2DkZisoN9h1dLa8Sn5sx0n</t>
         </is>
       </c>
       <c r="Z473" t="n">
-        <v>249840</v>
+        <v>233360</v>
       </c>
       <c r="AA473" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="474">
@@ -46640,41 +46640,41 @@
       <c r="H507" t="inlineStr"/>
       <c r="I507" t="inlineStr">
         <is>
-          <t>3rL9nFOkiqp3493H1DAFM4</t>
+          <t>4UWnGqJVp7TVpM0QLvZam7</t>
         </is>
       </c>
       <c r="J507" t="n">
-        <v>0.622</v>
+        <v>0.916</v>
       </c>
       <c r="K507" t="n">
-        <v>0.787</v>
+        <v>0.647</v>
       </c>
       <c r="L507" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M507" t="n">
-        <v>-4.766</v>
+        <v>-3.74</v>
       </c>
       <c r="N507" t="n">
         <v>0</v>
       </c>
       <c r="O507" t="n">
-        <v>0.076</v>
+        <v>0.04</v>
       </c>
       <c r="P507" t="n">
-        <v>0.119</v>
+        <v>0.247</v>
       </c>
       <c r="Q507" t="n">
         <v>0</v>
       </c>
       <c r="R507" t="n">
-        <v>0.06850000000000001</v>
+        <v>0.0665</v>
       </c>
       <c r="S507" t="n">
-        <v>0.653</v>
+        <v>0.927</v>
       </c>
       <c r="T507" t="n">
-        <v>115</v>
+        <v>100.047</v>
       </c>
       <c r="U507" t="inlineStr">
         <is>
@@ -46683,26 +46683,26 @@
       </c>
       <c r="V507" t="inlineStr">
         <is>
-          <t>3rL9nFOkiqp3493H1DAFM4</t>
+          <t>4UWnGqJVp7TVpM0QLvZam7</t>
         </is>
       </c>
       <c r="W507" t="inlineStr">
         <is>
-          <t>spotify:track:3rL9nFOkiqp3493H1DAFM4</t>
+          <t>spotify:track:4UWnGqJVp7TVpM0QLvZam7</t>
         </is>
       </c>
       <c r="X507" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3rL9nFOkiqp3493H1DAFM4</t>
+          <t>https://api.spotify.com/v1/tracks/4UWnGqJVp7TVpM0QLvZam7</t>
         </is>
       </c>
       <c r="Y507" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3rL9nFOkiqp3493H1DAFM4</t>
+          <t>https://api.spotify.com/v1/audio-analysis/4UWnGqJVp7TVpM0QLvZam7</t>
         </is>
       </c>
       <c r="Z507" t="n">
-        <v>174400</v>
+        <v>145241</v>
       </c>
       <c r="AA507" t="n">
         <v>4</v>
@@ -48096,41 +48096,41 @@
       <c r="H523" t="inlineStr"/>
       <c r="I523" t="inlineStr">
         <is>
-          <t>4p1mcA5wVKjzUfdxPoxSax</t>
+          <t>1pdckqLagXA7LFa5bhI8i4</t>
         </is>
       </c>
       <c r="J523" t="n">
-        <v>0.717</v>
+        <v>0.36</v>
       </c>
       <c r="K523" t="n">
-        <v>0.953</v>
+        <v>0.138</v>
       </c>
       <c r="L523" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M523" t="n">
-        <v>-1.255</v>
+        <v>-17.054</v>
       </c>
       <c r="N523" t="n">
         <v>1</v>
       </c>
       <c r="O523" t="n">
-        <v>0.08459999999999999</v>
+        <v>0.0401</v>
       </c>
       <c r="P523" t="n">
-        <v>0.153</v>
+        <v>0.975</v>
       </c>
       <c r="Q523" t="n">
-        <v>0</v>
+        <v>0.908</v>
       </c>
       <c r="R523" t="n">
-        <v>0.347</v>
+        <v>0.117</v>
       </c>
       <c r="S523" t="n">
-        <v>0.832</v>
+        <v>0.364</v>
       </c>
       <c r="T523" t="n">
-        <v>126.994</v>
+        <v>83.068</v>
       </c>
       <c r="U523" t="inlineStr">
         <is>
@@ -48139,29 +48139,29 @@
       </c>
       <c r="V523" t="inlineStr">
         <is>
-          <t>4p1mcA5wVKjzUfdxPoxSax</t>
+          <t>1pdckqLagXA7LFa5bhI8i4</t>
         </is>
       </c>
       <c r="W523" t="inlineStr">
         <is>
-          <t>spotify:track:4p1mcA5wVKjzUfdxPoxSax</t>
+          <t>spotify:track:1pdckqLagXA7LFa5bhI8i4</t>
         </is>
       </c>
       <c r="X523" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4p1mcA5wVKjzUfdxPoxSax</t>
+          <t>https://api.spotify.com/v1/tracks/1pdckqLagXA7LFa5bhI8i4</t>
         </is>
       </c>
       <c r="Y523" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4p1mcA5wVKjzUfdxPoxSax</t>
+          <t>https://api.spotify.com/v1/audio-analysis/1pdckqLagXA7LFa5bhI8i4</t>
         </is>
       </c>
       <c r="Z523" t="n">
-        <v>196827</v>
+        <v>208928</v>
       </c>
       <c r="AA523" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="524">
@@ -53303,41 +53303,41 @@
       <c r="H580" t="inlineStr"/>
       <c r="I580" t="inlineStr">
         <is>
-          <t>4InBqLg1DsZgWFCUZtm8GE</t>
+          <t>6x2XEXR6C7abyTZOGInSMb</t>
         </is>
       </c>
       <c r="J580" t="n">
-        <v>0.412</v>
+        <v>0.873</v>
       </c>
       <c r="K580" t="n">
-        <v>0.973</v>
+        <v>0.555</v>
       </c>
       <c r="L580" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M580" t="n">
-        <v>-2.663</v>
+        <v>-16.097</v>
       </c>
       <c r="N580" t="n">
         <v>0</v>
       </c>
       <c r="O580" t="n">
-        <v>0.183</v>
+        <v>0.187</v>
       </c>
       <c r="P580" t="n">
-        <v>0.009140000000000001</v>
+        <v>0.0179</v>
       </c>
       <c r="Q580" t="n">
-        <v>0</v>
+        <v>0.209</v>
       </c>
       <c r="R580" t="n">
-        <v>0.169</v>
+        <v>0.0485</v>
       </c>
       <c r="S580" t="n">
-        <v>0.544</v>
+        <v>0.8</v>
       </c>
       <c r="T580" t="n">
-        <v>168.023</v>
+        <v>149.978</v>
       </c>
       <c r="U580" t="inlineStr">
         <is>
@@ -53346,26 +53346,26 @@
       </c>
       <c r="V580" t="inlineStr">
         <is>
-          <t>4InBqLg1DsZgWFCUZtm8GE</t>
+          <t>6x2XEXR6C7abyTZOGInSMb</t>
         </is>
       </c>
       <c r="W580" t="inlineStr">
         <is>
-          <t>spotify:track:4InBqLg1DsZgWFCUZtm8GE</t>
+          <t>spotify:track:6x2XEXR6C7abyTZOGInSMb</t>
         </is>
       </c>
       <c r="X580" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/4InBqLg1DsZgWFCUZtm8GE</t>
+          <t>https://api.spotify.com/v1/tracks/6x2XEXR6C7abyTZOGInSMb</t>
         </is>
       </c>
       <c r="Y580" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/4InBqLg1DsZgWFCUZtm8GE</t>
+          <t>https://api.spotify.com/v1/audio-analysis/6x2XEXR6C7abyTZOGInSMb</t>
         </is>
       </c>
       <c r="Z580" t="n">
-        <v>203460</v>
+        <v>80256</v>
       </c>
       <c r="AA580" t="n">
         <v>4</v>
@@ -56306,41 +56306,41 @@
       <c r="H613" t="inlineStr"/>
       <c r="I613" t="inlineStr">
         <is>
-          <t>3ZQsO0kHzczapEdCrEYG4f</t>
+          <t>17yS6sY1uip6aAlbp6Ss6I</t>
         </is>
       </c>
       <c r="J613" t="n">
-        <v>0.805</v>
+        <v>0.545</v>
       </c>
       <c r="K613" t="n">
-        <v>0.827</v>
+        <v>0.777</v>
       </c>
       <c r="L613" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M613" t="n">
-        <v>-3.756</v>
+        <v>-5.003</v>
       </c>
       <c r="N613" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O613" t="n">
-        <v>0.059</v>
+        <v>0.07829999999999999</v>
       </c>
       <c r="P613" t="n">
-        <v>0.0432</v>
+        <v>0.123</v>
       </c>
       <c r="Q613" t="n">
-        <v>0.000133</v>
+        <v>0</v>
       </c>
       <c r="R613" t="n">
-        <v>0.0348</v>
+        <v>0.138</v>
       </c>
       <c r="S613" t="n">
-        <v>0.84</v>
+        <v>0.623</v>
       </c>
       <c r="T613" t="n">
-        <v>101.005</v>
+        <v>144.032</v>
       </c>
       <c r="U613" t="inlineStr">
         <is>
@@ -56349,26 +56349,26 @@
       </c>
       <c r="V613" t="inlineStr">
         <is>
-          <t>3ZQsO0kHzczapEdCrEYG4f</t>
+          <t>17yS6sY1uip6aAlbp6Ss6I</t>
         </is>
       </c>
       <c r="W613" t="inlineStr">
         <is>
-          <t>spotify:track:3ZQsO0kHzczapEdCrEYG4f</t>
+          <t>spotify:track:17yS6sY1uip6aAlbp6Ss6I</t>
         </is>
       </c>
       <c r="X613" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/3ZQsO0kHzczapEdCrEYG4f</t>
+          <t>https://api.spotify.com/v1/tracks/17yS6sY1uip6aAlbp6Ss6I</t>
         </is>
       </c>
       <c r="Y613" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/3ZQsO0kHzczapEdCrEYG4f</t>
+          <t>https://api.spotify.com/v1/audio-analysis/17yS6sY1uip6aAlbp6Ss6I</t>
         </is>
       </c>
       <c r="Z613" t="n">
-        <v>201067</v>
+        <v>190126</v>
       </c>
       <c r="AA613" t="n">
         <v>4</v>
@@ -58854,41 +58854,41 @@
       </c>
       <c r="I641" t="inlineStr">
         <is>
-          <t>2avKuMN2QXkaG9vvHa2JLt</t>
+          <t>56dtB7EzO7EneUgYwX8krC</t>
         </is>
       </c>
       <c r="J641" t="n">
-        <v>0.425</v>
+        <v>0.606</v>
       </c>
       <c r="K641" t="n">
-        <v>0.852</v>
+        <v>0.908</v>
       </c>
       <c r="L641" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="M641" t="n">
-        <v>-5.605</v>
+        <v>-5.736</v>
       </c>
       <c r="N641" t="n">
         <v>1</v>
       </c>
       <c r="O641" t="n">
-        <v>0.0461</v>
+        <v>0.037</v>
       </c>
       <c r="P641" t="n">
-        <v>0.0174</v>
+        <v>0.00532</v>
       </c>
       <c r="Q641" t="n">
-        <v>0.311</v>
+        <v>0.823</v>
       </c>
       <c r="R641" t="n">
-        <v>0.0935</v>
+        <v>0.245</v>
       </c>
       <c r="S641" t="n">
-        <v>0.499</v>
+        <v>0.773</v>
       </c>
       <c r="T641" t="n">
-        <v>101.97</v>
+        <v>130.12</v>
       </c>
       <c r="U641" t="inlineStr">
         <is>
@@ -58897,26 +58897,26 @@
       </c>
       <c r="V641" t="inlineStr">
         <is>
-          <t>2avKuMN2QXkaG9vvHa2JLt</t>
+          <t>56dtB7EzO7EneUgYwX8krC</t>
         </is>
       </c>
       <c r="W641" t="inlineStr">
         <is>
-          <t>spotify:track:2avKuMN2QXkaG9vvHa2JLt</t>
+          <t>spotify:track:56dtB7EzO7EneUgYwX8krC</t>
         </is>
       </c>
       <c r="X641" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2avKuMN2QXkaG9vvHa2JLt</t>
+          <t>https://api.spotify.com/v1/tracks/56dtB7EzO7EneUgYwX8krC</t>
         </is>
       </c>
       <c r="Y641" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2avKuMN2QXkaG9vvHa2JLt</t>
+          <t>https://api.spotify.com/v1/audio-analysis/56dtB7EzO7EneUgYwX8krC</t>
         </is>
       </c>
       <c r="Z641" t="n">
-        <v>321040</v>
+        <v>159173</v>
       </c>
       <c r="AA641" t="n">
         <v>4</v>
@@ -59400,41 +59400,41 @@
       </c>
       <c r="I647" t="inlineStr">
         <is>
-          <t>05m2aME4QqRmKCJKbYK5j2</t>
+          <t>16Azhyv8164hYxI8Ax3F5k</t>
         </is>
       </c>
       <c r="J647" t="n">
-        <v>0.189</v>
+        <v>0.834</v>
       </c>
       <c r="K647" t="n">
-        <v>0.299</v>
+        <v>0.6</v>
       </c>
       <c r="L647" t="n">
         <v>5</v>
       </c>
       <c r="M647" t="n">
-        <v>-14.592</v>
+        <v>-5.433</v>
       </c>
       <c r="N647" t="n">
         <v>1</v>
       </c>
       <c r="O647" t="n">
-        <v>0.0379</v>
+        <v>0.0313</v>
       </c>
       <c r="P647" t="n">
-        <v>0.95</v>
+        <v>0.245</v>
       </c>
       <c r="Q647" t="n">
-        <v>0.0387</v>
+        <v>0</v>
       </c>
       <c r="R647" t="n">
-        <v>0.068</v>
+        <v>0.0694</v>
       </c>
       <c r="S647" t="n">
-        <v>0.0379</v>
+        <v>0.694</v>
       </c>
       <c r="T647" t="n">
-        <v>75.262</v>
+        <v>125.954</v>
       </c>
       <c r="U647" t="inlineStr">
         <is>
@@ -59443,29 +59443,29 @@
       </c>
       <c r="V647" t="inlineStr">
         <is>
-          <t>05m2aME4QqRmKCJKbYK5j2</t>
+          <t>16Azhyv8164hYxI8Ax3F5k</t>
         </is>
       </c>
       <c r="W647" t="inlineStr">
         <is>
-          <t>spotify:track:05m2aME4QqRmKCJKbYK5j2</t>
+          <t>spotify:track:16Azhyv8164hYxI8Ax3F5k</t>
         </is>
       </c>
       <c r="X647" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/05m2aME4QqRmKCJKbYK5j2</t>
+          <t>https://api.spotify.com/v1/tracks/16Azhyv8164hYxI8Ax3F5k</t>
         </is>
       </c>
       <c r="Y647" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/05m2aME4QqRmKCJKbYK5j2</t>
+          <t>https://api.spotify.com/v1/audio-analysis/16Azhyv8164hYxI8Ax3F5k</t>
         </is>
       </c>
       <c r="Z647" t="n">
-        <v>307962</v>
+        <v>131429</v>
       </c>
       <c r="AA647" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="648">
@@ -61129,41 +61129,41 @@
       </c>
       <c r="I666" t="inlineStr">
         <is>
-          <t>2dGNWBuNUlNTRZeWP01BYl</t>
+          <t>6h7jn2jE2EqJadOkDXsDJh</t>
         </is>
       </c>
       <c r="J666" t="n">
-        <v>0.519</v>
+        <v>0.652</v>
       </c>
       <c r="K666" t="n">
-        <v>0.545</v>
+        <v>0.671</v>
       </c>
       <c r="L666" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M666" t="n">
-        <v>-5.55</v>
+        <v>-7.254</v>
       </c>
       <c r="N666" t="n">
         <v>1</v>
       </c>
       <c r="O666" t="n">
-        <v>0.0317</v>
+        <v>0.0446</v>
       </c>
       <c r="P666" t="n">
-        <v>0.421</v>
+        <v>0.492</v>
       </c>
       <c r="Q666" t="n">
-        <v>0</v>
+        <v>0.0863</v>
       </c>
       <c r="R666" t="n">
-        <v>0.136</v>
+        <v>0.0873</v>
       </c>
       <c r="S666" t="n">
-        <v>0.227</v>
+        <v>0.249</v>
       </c>
       <c r="T666" t="n">
-        <v>143.184</v>
+        <v>91.518</v>
       </c>
       <c r="U666" t="inlineStr">
         <is>
@@ -61172,26 +61172,26 @@
       </c>
       <c r="V666" t="inlineStr">
         <is>
-          <t>2dGNWBuNUlNTRZeWP01BYl</t>
+          <t>6h7jn2jE2EqJadOkDXsDJh</t>
         </is>
       </c>
       <c r="W666" t="inlineStr">
         <is>
-          <t>spotify:track:2dGNWBuNUlNTRZeWP01BYl</t>
+          <t>spotify:track:6h7jn2jE2EqJadOkDXsDJh</t>
         </is>
       </c>
       <c r="X666" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2dGNWBuNUlNTRZeWP01BYl</t>
+          <t>https://api.spotify.com/v1/tracks/6h7jn2jE2EqJadOkDXsDJh</t>
         </is>
       </c>
       <c r="Y666" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2dGNWBuNUlNTRZeWP01BYl</t>
+          <t>https://api.spotify.com/v1/audio-analysis/6h7jn2jE2EqJadOkDXsDJh</t>
         </is>
       </c>
       <c r="Z666" t="n">
-        <v>258247</v>
+        <v>179226</v>
       </c>
       <c r="AA666" t="n">
         <v>4</v>
@@ -61220,41 +61220,41 @@
       </c>
       <c r="I667" t="inlineStr">
         <is>
-          <t>6kH1sKkvgN4Yikake52glq</t>
+          <t>5d61V7Jtc82vKxi3NRP9Ky</t>
         </is>
       </c>
       <c r="J667" t="n">
-        <v>0.602</v>
+        <v>0.658</v>
       </c>
       <c r="K667" t="n">
-        <v>0.947</v>
+        <v>0.472</v>
       </c>
       <c r="L667" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M667" t="n">
-        <v>-1.613</v>
+        <v>-5.552</v>
       </c>
       <c r="N667" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O667" t="n">
-        <v>0.0615</v>
+        <v>0.458</v>
       </c>
       <c r="P667" t="n">
-        <v>0.182</v>
+        <v>0.222</v>
       </c>
       <c r="Q667" t="n">
-        <v>1.47e-05</v>
+        <v>1.48e-06</v>
       </c>
       <c r="R667" t="n">
-        <v>0.132</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="S667" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.438</v>
       </c>
       <c r="T667" t="n">
-        <v>110.055</v>
+        <v>207.91</v>
       </c>
       <c r="U667" t="inlineStr">
         <is>
@@ -61263,26 +61263,26 @@
       </c>
       <c r="V667" t="inlineStr">
         <is>
-          <t>6kH1sKkvgN4Yikake52glq</t>
+          <t>5d61V7Jtc82vKxi3NRP9Ky</t>
         </is>
       </c>
       <c r="W667" t="inlineStr">
         <is>
-          <t>spotify:track:6kH1sKkvgN4Yikake52glq</t>
+          <t>spotify:track:5d61V7Jtc82vKxi3NRP9Ky</t>
         </is>
       </c>
       <c r="X667" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/6kH1sKkvgN4Yikake52glq</t>
+          <t>https://api.spotify.com/v1/tracks/5d61V7Jtc82vKxi3NRP9Ky</t>
         </is>
       </c>
       <c r="Y667" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/6kH1sKkvgN4Yikake52glq</t>
+          <t>https://api.spotify.com/v1/audio-analysis/5d61V7Jtc82vKxi3NRP9Ky</t>
         </is>
       </c>
       <c r="Z667" t="n">
-        <v>189933</v>
+        <v>129750</v>
       </c>
       <c r="AA667" t="n">
         <v>4</v>
@@ -62858,41 +62858,41 @@
       </c>
       <c r="I685" t="inlineStr">
         <is>
-          <t>5Qv2Nby1xTr9pQyjkrc94J</t>
+          <t>0QXJbWSTllPExeX9jXbh2B</t>
         </is>
       </c>
       <c r="J685" t="n">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="K685" t="n">
-        <v>0.478</v>
+        <v>0.449</v>
       </c>
       <c r="L685" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M685" t="n">
-        <v>-8.689</v>
+        <v>-10.323</v>
       </c>
       <c r="N685" t="n">
         <v>0</v>
       </c>
       <c r="O685" t="n">
-        <v>0.0355</v>
+        <v>0.103</v>
       </c>
       <c r="P685" t="n">
-        <v>0.531</v>
+        <v>0.406</v>
       </c>
       <c r="Q685" t="n">
-        <v>0.428</v>
+        <v>0</v>
       </c>
       <c r="R685" t="n">
-        <v>0.138</v>
+        <v>0.118</v>
       </c>
       <c r="S685" t="n">
-        <v>0.0997</v>
+        <v>0.339</v>
       </c>
       <c r="T685" t="n">
-        <v>88.014</v>
+        <v>140.883</v>
       </c>
       <c r="U685" t="inlineStr">
         <is>
@@ -62901,26 +62901,26 @@
       </c>
       <c r="V685" t="inlineStr">
         <is>
-          <t>5Qv2Nby1xTr9pQyjkrc94J</t>
+          <t>0QXJbWSTllPExeX9jXbh2B</t>
         </is>
       </c>
       <c r="W685" t="inlineStr">
         <is>
-          <t>spotify:track:5Qv2Nby1xTr9pQyjkrc94J</t>
+          <t>spotify:track:0QXJbWSTllPExeX9jXbh2B</t>
         </is>
       </c>
       <c r="X685" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/5Qv2Nby1xTr9pQyjkrc94J</t>
+          <t>https://api.spotify.com/v1/tracks/0QXJbWSTllPExeX9jXbh2B</t>
         </is>
       </c>
       <c r="Y685" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/5Qv2Nby1xTr9pQyjkrc94J</t>
+          <t>https://api.spotify.com/v1/audio-analysis/0QXJbWSTllPExeX9jXbh2B</t>
         </is>
       </c>
       <c r="Z685" t="n">
-        <v>228747</v>
+        <v>204700</v>
       </c>
       <c r="AA685" t="n">
         <v>4</v>
@@ -64496,41 +64496,41 @@
       </c>
       <c r="I703" t="inlineStr">
         <is>
-          <t>2ZG2MBGBeBb6xdAy0Th9F9</t>
+          <t>5DvtItAqwyjx4mpw4i4fNC</t>
         </is>
       </c>
       <c r="J703" t="n">
-        <v>0.623</v>
+        <v>0.622</v>
       </c>
       <c r="K703" t="n">
-        <v>0.9</v>
+        <v>0.907</v>
       </c>
       <c r="L703" t="n">
         <v>2</v>
       </c>
       <c r="M703" t="n">
-        <v>-2.441</v>
+        <v>-2.439</v>
       </c>
       <c r="N703" t="n">
         <v>0</v>
       </c>
       <c r="O703" t="n">
-        <v>0.0517</v>
+        <v>0.0507</v>
       </c>
       <c r="P703" t="n">
-        <v>0.216</v>
+        <v>0.218</v>
       </c>
       <c r="Q703" t="n">
         <v>0</v>
       </c>
       <c r="R703" t="n">
-        <v>0.0834</v>
+        <v>0.08550000000000001</v>
       </c>
       <c r="S703" t="n">
-        <v>0.859</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="T703" t="n">
-        <v>124.958</v>
+        <v>124.943</v>
       </c>
       <c r="U703" t="inlineStr">
         <is>
@@ -64539,22 +64539,22 @@
       </c>
       <c r="V703" t="inlineStr">
         <is>
-          <t>2ZG2MBGBeBb6xdAy0Th9F9</t>
+          <t>5DvtItAqwyjx4mpw4i4fNC</t>
         </is>
       </c>
       <c r="W703" t="inlineStr">
         <is>
-          <t>spotify:track:2ZG2MBGBeBb6xdAy0Th9F9</t>
+          <t>spotify:track:5DvtItAqwyjx4mpw4i4fNC</t>
         </is>
       </c>
       <c r="X703" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2ZG2MBGBeBb6xdAy0Th9F9</t>
+          <t>https://api.spotify.com/v1/tracks/5DvtItAqwyjx4mpw4i4fNC</t>
         </is>
       </c>
       <c r="Y703" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2ZG2MBGBeBb6xdAy0Th9F9</t>
+          <t>https://api.spotify.com/v1/audio-analysis/5DvtItAqwyjx4mpw4i4fNC</t>
         </is>
       </c>
       <c r="Z703" t="n">
@@ -64587,41 +64587,41 @@
       </c>
       <c r="I704" t="inlineStr">
         <is>
-          <t>0FMkt7EXvAEdGg24cVnwWe</t>
+          <t>53SSnDsAYRJX0dVtnyJbwX</t>
         </is>
       </c>
       <c r="J704" t="n">
-        <v>0.705</v>
+        <v>0.704</v>
       </c>
       <c r="K704" t="n">
-        <v>0.967</v>
+        <v>0.968</v>
       </c>
       <c r="L704" t="n">
         <v>7</v>
       </c>
       <c r="M704" t="n">
-        <v>-1.609</v>
+        <v>-1.452</v>
       </c>
       <c r="N704" t="n">
         <v>0</v>
       </c>
       <c r="O704" t="n">
-        <v>0.0692</v>
+        <v>0.07149999999999999</v>
       </c>
       <c r="P704" t="n">
-        <v>0.06320000000000001</v>
+        <v>0.0604</v>
       </c>
       <c r="Q704" t="n">
         <v>0</v>
       </c>
       <c r="R704" t="n">
-        <v>0.15</v>
+        <v>0.148</v>
       </c>
       <c r="S704" t="n">
-        <v>0.806</v>
+        <v>0.786</v>
       </c>
       <c r="T704" t="n">
-        <v>122</v>
+        <v>122.006</v>
       </c>
       <c r="U704" t="inlineStr">
         <is>
@@ -64630,22 +64630,22 @@
       </c>
       <c r="V704" t="inlineStr">
         <is>
-          <t>0FMkt7EXvAEdGg24cVnwWe</t>
+          <t>53SSnDsAYRJX0dVtnyJbwX</t>
         </is>
       </c>
       <c r="W704" t="inlineStr">
         <is>
-          <t>spotify:track:0FMkt7EXvAEdGg24cVnwWe</t>
+          <t>spotify:track:53SSnDsAYRJX0dVtnyJbwX</t>
         </is>
       </c>
       <c r="X704" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/0FMkt7EXvAEdGg24cVnwWe</t>
+          <t>https://api.spotify.com/v1/tracks/53SSnDsAYRJX0dVtnyJbwX</t>
         </is>
       </c>
       <c r="Y704" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/0FMkt7EXvAEdGg24cVnwWe</t>
+          <t>https://api.spotify.com/v1/audio-analysis/53SSnDsAYRJX0dVtnyJbwX</t>
         </is>
       </c>
       <c r="Z704" t="n">
@@ -64678,26 +64678,26 @@
       </c>
       <c r="I705" t="inlineStr">
         <is>
-          <t>7qDbAc6xMW07T7yyMnQqS8</t>
+          <t>7b2Ppk9bjhT1EFnRNb7mxL</t>
         </is>
       </c>
       <c r="J705" t="n">
-        <v>0.764</v>
+        <v>0.762</v>
       </c>
       <c r="K705" t="n">
-        <v>0.836</v>
+        <v>0.841</v>
       </c>
       <c r="L705" t="n">
         <v>1</v>
       </c>
       <c r="M705" t="n">
-        <v>-2.868</v>
+        <v>-2.836</v>
       </c>
       <c r="N705" t="n">
         <v>1</v>
       </c>
       <c r="O705" t="n">
-        <v>0.0396</v>
+        <v>0.0424</v>
       </c>
       <c r="P705" t="n">
         <v>0.208</v>
@@ -64706,13 +64706,13 @@
         <v>0</v>
       </c>
       <c r="R705" t="n">
-        <v>0.234</v>
+        <v>0.267</v>
       </c>
       <c r="S705" t="n">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="T705" t="n">
-        <v>111.934</v>
+        <v>111.947</v>
       </c>
       <c r="U705" t="inlineStr">
         <is>
@@ -64721,22 +64721,22 @@
       </c>
       <c r="V705" t="inlineStr">
         <is>
-          <t>7qDbAc6xMW07T7yyMnQqS8</t>
+          <t>7b2Ppk9bjhT1EFnRNb7mxL</t>
         </is>
       </c>
       <c r="W705" t="inlineStr">
         <is>
-          <t>spotify:track:7qDbAc6xMW07T7yyMnQqS8</t>
+          <t>spotify:track:7b2Ppk9bjhT1EFnRNb7mxL</t>
         </is>
       </c>
       <c r="X705" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/7qDbAc6xMW07T7yyMnQqS8</t>
+          <t>https://api.spotify.com/v1/tracks/7b2Ppk9bjhT1EFnRNb7mxL</t>
         </is>
       </c>
       <c r="Y705" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/7qDbAc6xMW07T7yyMnQqS8</t>
+          <t>https://api.spotify.com/v1/audio-analysis/7b2Ppk9bjhT1EFnRNb7mxL</t>
         </is>
       </c>
       <c r="Z705" t="n">
@@ -69408,41 +69408,41 @@
       </c>
       <c r="I757" t="inlineStr">
         <is>
-          <t>1e7eOq89QU6vGYCJp9yW2L</t>
+          <t>31ihTxEFH8iLwYuXiXTyK8</t>
         </is>
       </c>
       <c r="J757" t="n">
-        <v>0.453</v>
+        <v>0.447</v>
       </c>
       <c r="K757" t="n">
-        <v>0.849</v>
+        <v>0.852</v>
       </c>
       <c r="L757" t="n">
         <v>6</v>
       </c>
       <c r="M757" t="n">
-        <v>-1.337</v>
+        <v>-1.35</v>
       </c>
       <c r="N757" t="n">
         <v>0</v>
       </c>
       <c r="O757" t="n">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
       <c r="P757" t="n">
-        <v>0.428</v>
+        <v>0.411</v>
       </c>
       <c r="Q757" t="n">
         <v>0</v>
       </c>
       <c r="R757" t="n">
-        <v>0.1</v>
+        <v>0.101</v>
       </c>
       <c r="S757" t="n">
-        <v>0.638</v>
+        <v>0.589</v>
       </c>
       <c r="T757" t="n">
-        <v>173.917</v>
+        <v>173.915</v>
       </c>
       <c r="U757" t="inlineStr">
         <is>
@@ -69451,22 +69451,22 @@
       </c>
       <c r="V757" t="inlineStr">
         <is>
-          <t>1e7eOq89QU6vGYCJp9yW2L</t>
+          <t>31ihTxEFH8iLwYuXiXTyK8</t>
         </is>
       </c>
       <c r="W757" t="inlineStr">
         <is>
-          <t>spotify:track:1e7eOq89QU6vGYCJp9yW2L</t>
+          <t>spotify:track:31ihTxEFH8iLwYuXiXTyK8</t>
         </is>
       </c>
       <c r="X757" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/1e7eOq89QU6vGYCJp9yW2L</t>
+          <t>https://api.spotify.com/v1/tracks/31ihTxEFH8iLwYuXiXTyK8</t>
         </is>
       </c>
       <c r="Y757" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/1e7eOq89QU6vGYCJp9yW2L</t>
+          <t>https://api.spotify.com/v1/audio-analysis/31ihTxEFH8iLwYuXiXTyK8</t>
         </is>
       </c>
       <c r="Z757" t="n">
@@ -69863,41 +69863,41 @@
       </c>
       <c r="I762" t="inlineStr">
         <is>
-          <t>2pGmF3K8HnvQXMEQBUHNM1</t>
+          <t>6QGbnTI040wEqJcUit8jOw</t>
         </is>
       </c>
       <c r="J762" t="n">
-        <v>0.721</v>
+        <v>0.621</v>
       </c>
       <c r="K762" t="n">
-        <v>0.738</v>
+        <v>0.306</v>
       </c>
       <c r="L762" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M762" t="n">
-        <v>-9.471</v>
+        <v>-15.359</v>
       </c>
       <c r="N762" t="n">
         <v>0</v>
       </c>
       <c r="O762" t="n">
-        <v>0.215</v>
+        <v>0.0759</v>
       </c>
       <c r="P762" t="n">
-        <v>0.0107</v>
+        <v>0.749</v>
       </c>
       <c r="Q762" t="n">
-        <v>0.641</v>
+        <v>2.46e-05</v>
       </c>
       <c r="R762" t="n">
-        <v>0.117</v>
+        <v>0.349</v>
       </c>
       <c r="S762" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.526</v>
       </c>
       <c r="T762" t="n">
-        <v>127.985</v>
+        <v>78.746</v>
       </c>
       <c r="U762" t="inlineStr">
         <is>
@@ -69906,26 +69906,26 @@
       </c>
       <c r="V762" t="inlineStr">
         <is>
-          <t>2pGmF3K8HnvQXMEQBUHNM1</t>
+          <t>6QGbnTI040wEqJcUit8jOw</t>
         </is>
       </c>
       <c r="W762" t="inlineStr">
         <is>
-          <t>spotify:track:2pGmF3K8HnvQXMEQBUHNM1</t>
+          <t>spotify:track:6QGbnTI040wEqJcUit8jOw</t>
         </is>
       </c>
       <c r="X762" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2pGmF3K8HnvQXMEQBUHNM1</t>
+          <t>https://api.spotify.com/v1/tracks/6QGbnTI040wEqJcUit8jOw</t>
         </is>
       </c>
       <c r="Y762" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2pGmF3K8HnvQXMEQBUHNM1</t>
+          <t>https://api.spotify.com/v1/audio-analysis/6QGbnTI040wEqJcUit8jOw</t>
         </is>
       </c>
       <c r="Z762" t="n">
-        <v>174728</v>
+        <v>260200</v>
       </c>
       <c r="AA762" t="n">
         <v>4</v>
@@ -75786,41 +75786,41 @@
       </c>
       <c r="I827" t="inlineStr">
         <is>
-          <t>7xAACq6jlGqXw4bNCTYcm6</t>
+          <t>4dgeadQAd4wEP6NAPoRLZt</t>
         </is>
       </c>
       <c r="J827" t="n">
-        <v>0.75</v>
+        <v>0.696</v>
       </c>
       <c r="K827" t="n">
-        <v>0.914</v>
+        <v>0.008540000000000001</v>
       </c>
       <c r="L827" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M827" t="n">
-        <v>-1.819</v>
+        <v>-28.699</v>
       </c>
       <c r="N827" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O827" t="n">
-        <v>0.0518</v>
+        <v>0.07580000000000001</v>
       </c>
       <c r="P827" t="n">
-        <v>0.0323</v>
+        <v>0.981</v>
       </c>
       <c r="Q827" t="n">
-        <v>0</v>
+        <v>0.945</v>
       </c>
       <c r="R827" t="n">
         <v>0.107</v>
       </c>
       <c r="S827" t="n">
-        <v>0.866</v>
+        <v>0.501</v>
       </c>
       <c r="T827" t="n">
-        <v>125.034</v>
+        <v>67.991</v>
       </c>
       <c r="U827" t="inlineStr">
         <is>
@@ -75829,26 +75829,26 @@
       </c>
       <c r="V827" t="inlineStr">
         <is>
-          <t>7xAACq6jlGqXw4bNCTYcm6</t>
+          <t>4dgeadQAd4wEP6NAPoRLZt</t>
         </is>
       </c>
       <c r="W827" t="inlineStr">
         <is>
-          <t>spotify:track:7xAACq6jlGqXw4bNCTYcm6</t>
+          <t>spotify:track:4dgeadQAd4wEP6NAPoRLZt</t>
         </is>
       </c>
       <c r="X827" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/7xAACq6jlGqXw4bNCTYcm6</t>
+          <t>https://api.spotify.com/v1/tracks/4dgeadQAd4wEP6NAPoRLZt</t>
         </is>
       </c>
       <c r="Y827" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/7xAACq6jlGqXw4bNCTYcm6</t>
+          <t>https://api.spotify.com/v1/audio-analysis/4dgeadQAd4wEP6NAPoRLZt</t>
         </is>
       </c>
       <c r="Z827" t="n">
-        <v>233987</v>
+        <v>69669</v>
       </c>
       <c r="AA827" t="n">
         <v>4</v>
@@ -77697,41 +77697,41 @@
       </c>
       <c r="I848" t="inlineStr">
         <is>
-          <t>5RENkTP0he793Basw1Stto</t>
+          <t>2wTwhiAm1via7YfhzWgoGZ</t>
         </is>
       </c>
       <c r="J848" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.704</v>
       </c>
       <c r="K848" t="n">
-        <v>0.8129999999999999</v>
+        <v>0.852</v>
       </c>
       <c r="L848" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M848" t="n">
-        <v>-5.901</v>
+        <v>-4.13</v>
       </c>
       <c r="N848" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O848" t="n">
-        <v>0.0434</v>
+        <v>0.0427</v>
       </c>
       <c r="P848" t="n">
-        <v>0.0012</v>
+        <v>0.0339</v>
       </c>
       <c r="Q848" t="n">
-        <v>5.96e-05</v>
+        <v>0</v>
       </c>
       <c r="R848" t="n">
-        <v>0.246</v>
+        <v>0.125</v>
       </c>
       <c r="S848" t="n">
-        <v>0.584</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="T848" t="n">
-        <v>124.975</v>
+        <v>147.944</v>
       </c>
       <c r="U848" t="inlineStr">
         <is>
@@ -77740,26 +77740,26 @@
       </c>
       <c r="V848" t="inlineStr">
         <is>
-          <t>5RENkTP0he793Basw1Stto</t>
+          <t>2wTwhiAm1via7YfhzWgoGZ</t>
         </is>
       </c>
       <c r="W848" t="inlineStr">
         <is>
-          <t>spotify:track:5RENkTP0he793Basw1Stto</t>
+          <t>spotify:track:2wTwhiAm1via7YfhzWgoGZ</t>
         </is>
       </c>
       <c r="X848" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/5RENkTP0he793Basw1Stto</t>
+          <t>https://api.spotify.com/v1/tracks/2wTwhiAm1via7YfhzWgoGZ</t>
         </is>
       </c>
       <c r="Y848" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/5RENkTP0he793Basw1Stto</t>
+          <t>https://api.spotify.com/v1/audio-analysis/2wTwhiAm1via7YfhzWgoGZ</t>
         </is>
       </c>
       <c r="Z848" t="n">
-        <v>198827</v>
+        <v>248027</v>
       </c>
       <c r="AA848" t="n">
         <v>4</v>
@@ -79062,7 +79062,7 @@
       </c>
       <c r="I863" t="inlineStr">
         <is>
-          <t>2EmcTFQ1rM11wp2ztsXTHa</t>
+          <t>6wH3AP7b01vpzKYRJhreMy</t>
         </is>
       </c>
       <c r="J863" t="n">
@@ -79105,22 +79105,22 @@
       </c>
       <c r="V863" t="inlineStr">
         <is>
-          <t>2EmcTFQ1rM11wp2ztsXTHa</t>
+          <t>6wH3AP7b01vpzKYRJhreMy</t>
         </is>
       </c>
       <c r="W863" t="inlineStr">
         <is>
-          <t>spotify:track:2EmcTFQ1rM11wp2ztsXTHa</t>
+          <t>spotify:track:6wH3AP7b01vpzKYRJhreMy</t>
         </is>
       </c>
       <c r="X863" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/tracks/2EmcTFQ1rM11wp2ztsXTHa</t>
+          <t>https://api.spotify.com/v1/tracks/6wH3AP7b01vpzKYRJhreMy</t>
         </is>
       </c>
       <c r="Y863" t="inlineStr">
         <is>
-          <t>https://api.spotify.com/v1/audio-analysis/2EmcTFQ1rM11wp2ztsXTHa</t>
+          <t>https://api.spotify.com/v1/audio-analysis/6wH3AP7b01vpzKYRJhreMy</t>
         </is>
       </c>
       <c r="Z863" t="n">

</xml_diff>